<commit_message>
Fixed TB Form PDF download
</commit_message>
<xml_diff>
--- a/public/files/tb-excel-form.xlsx
+++ b/public/files/tb-excel-form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Sites/localhost/ept/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472D1794-D238-3B43-AEF1-D1396EC40497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE5745-7305-2A4B-9850-49B5F1FF9597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="491" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Country:</t>
   </si>
@@ -95,12 +95,6 @@
     <t>ePT Username</t>
   </si>
   <si>
-    <t>Assay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      MTB/RIF             MTB/RIF Ultra</t>
-  </si>
-  <si>
     <t>Cartridge Lot Number</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
   </si>
   <si>
     <t>DETECTED</t>
-  </si>
-  <si>
-    <t>Indeterminate</t>
   </si>
   <si>
     <t xml:space="preserve"> INVALID </t>
@@ -355,40 +346,25 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This form is for your site's proficiency test records only.  All results must be submitted on ePT at </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>http://tbpt.org</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> using your username and password above. </t>
-    </r>
+    <t>Proficiency Test Panel ID:</t>
   </si>
   <si>
-    <t>Detected</t>
+    <t>INVALID</t>
   </si>
   <si>
-    <t>Invalid</t>
+    <t>INDETERMINATE</t>
   </si>
   <si>
-    <t>Error</t>
+    <t xml:space="preserve">This form is for your site's proficiency test records only.  All results must be submitted on ePT using your username and password above. </t>
   </si>
   <si>
-    <t>Proficiency Test Panel ID:</t>
+    <t>MTB/RIF Ultra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTB/RIF             </t>
+  </si>
+  <si>
+    <t>Assay (Tick One)</t>
   </si>
 </sst>
 </file>
@@ -451,12 +427,6 @@
     </font>
     <font>
       <b/>
-      <sz val="7"/>
-      <color theme="1"/>
-      <name val="Aharoni"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10.5"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -509,6 +479,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -548,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -632,34 +610,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -718,14 +668,14 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -734,7 +684,7 @@
       <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -747,10 +697,12 @@
       <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -766,22 +718,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -790,28 +727,69 @@
       <left style="thick">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -823,10 +801,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -838,10 +814,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -853,90 +827,8 @@
       <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -968,93 +860,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1110,11 +915,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1147,88 +987,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1240,48 +1053,24 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1300,24 +1089,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1330,27 +1107,115 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1360,175 +1225,106 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2297,7 +2093,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4725299" y="4161270"/>
+          <a:off x="4292939" y="4068821"/>
           <a:ext cx="192578" cy="166255"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -5673,16 +5469,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>122035</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>59766</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>137432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>204932</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>131139</xdr:rowOff>
+      <xdr:colOff>204933</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104588</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5697,8 +5493,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6700635" y="5458732"/>
-          <a:ext cx="1771997" cy="908107"/>
+          <a:off x="5483413" y="5232373"/>
+          <a:ext cx="2879402" cy="699274"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -5741,16 +5537,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>26988</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>52294</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>2571</xdr:rowOff>
+      <xdr:rowOff>2572</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>371764</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>84515</xdr:rowOff>
+      <xdr:colOff>371765</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>97118</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5765,8 +5561,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6605588" y="5666771"/>
-          <a:ext cx="1563976" cy="462944"/>
+          <a:off x="5475941" y="5441160"/>
+          <a:ext cx="2635353" cy="288782"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5794,7 +5590,7 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr"/>
+          <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Please</a:t>
@@ -6159,23 +5955,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>41271</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>39688</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>42174</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>49645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>233849</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>205943</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>234752</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="147" name="Oval 146">
+        <xdr:cNvPr id="2" name="Oval 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5195BF6C-1568-475B-BAA7-B711A7F0A841}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E52BE8C-0920-0642-8528-A99CF296CD97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6183,7 +5979,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7381871" y="1792288"/>
+          <a:off x="4292939" y="4068821"/>
           <a:ext cx="192578" cy="166255"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -6227,23 +6023,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>196846</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>41275</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>42174</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>49645</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>371961</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>207530</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>234752</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="148" name="Oval 147">
+        <xdr:cNvPr id="5" name="Oval 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6431EEC8-ED44-497D-A748-071922F48C69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D709FF2-61A6-C341-A132-8ADC9540D20F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6251,8 +6047,212 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8147046" y="1793875"/>
-          <a:ext cx="175115" cy="166255"/>
+          <a:off x="4292939" y="4337763"/>
+          <a:ext cx="192578" cy="166255"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>42174</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>49645</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>234752</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EBD989C-7129-224C-A859-2D8FD028E6E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4292939" y="4606704"/>
+          <a:ext cx="192578" cy="166255"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>42174</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>49645</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>234752</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D9BD1EA-9410-2A4B-AABF-0D05AF080CD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4292939" y="4875645"/>
+          <a:ext cx="192578" cy="166255"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>42174</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>49645</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>234752</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Oval 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDCD683B-5B08-5F41-A714-2B970322E804}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4292939" y="5144586"/>
+          <a:ext cx="192578" cy="166255"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6629,10 +6629,10 @@
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="14" width="3.5" customWidth="1"/>
     <col min="15" max="15" width="8.33203125" customWidth="1"/>
-    <col min="16" max="16" width="7" customWidth="1"/>
-    <col min="17" max="17" width="7.33203125" customWidth="1"/>
+    <col min="16" max="16" width="6" customWidth="1"/>
+    <col min="17" max="17" width="6.1640625" customWidth="1"/>
     <col min="18" max="18" width="5.83203125" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" customWidth="1"/>
+    <col min="19" max="19" width="4.33203125" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
     <col min="21" max="21" width="5.5" customWidth="1"/>
     <col min="22" max="22" width="3.6640625" customWidth="1"/>
@@ -6640,598 +6640,615 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="137" t="s">
-        <v>55</v>
+      <c r="A1" s="123" t="s">
+        <v>48</v>
       </c>
-      <c r="B1" s="137"/>
-      <c r="C1" s="137"/>
-      <c r="D1" s="137"/>
-      <c r="E1" s="137"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="H1" s="137"/>
-      <c r="I1" s="137"/>
-      <c r="J1" s="138" t="s">
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="139" t="s">
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="139"/>
-      <c r="T1" s="139"/>
-      <c r="U1" s="139"/>
-      <c r="V1" s="139"/>
-      <c r="W1" s="139"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="74"/>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
-      <c r="X2" s="52"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="38"/>
     </row>
-    <row r="3" spans="1:24" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="91" t="s">
+    <row r="3" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="91"/>
-      <c r="S3" s="91"/>
-      <c r="T3" s="91"/>
-      <c r="U3" s="91"/>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
-      <c r="X3" s="52"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="38"/>
     </row>
-    <row r="4" spans="1:24" ht="8.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="91"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="91"/>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
-      <c r="S4" s="91"/>
-      <c r="T4" s="91"/>
-      <c r="U4" s="91"/>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91"/>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A4" s="100"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="100"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="100"/>
+      <c r="V4" s="100"/>
+      <c r="W4" s="100"/>
     </row>
-    <row r="5" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
+    <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="77" t="s">
+      <c r="B5" s="101"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="111"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="79"/>
-      <c r="S5" s="77" t="s">
+      <c r="P5" s="98"/>
+      <c r="Q5" s="98"/>
+      <c r="R5" s="98"/>
+      <c r="S5" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="78"/>
-      <c r="U5" s="78"/>
-      <c r="V5" s="78"/>
-      <c r="W5" s="79"/>
+      <c r="T5" s="98"/>
+      <c r="U5" s="98"/>
+      <c r="V5" s="98"/>
+      <c r="W5" s="98"/>
     </row>
-    <row r="6" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="82"/>
-      <c r="S6" s="122"/>
-      <c r="T6" s="123"/>
-      <c r="U6" s="123"/>
-      <c r="V6" s="123"/>
-      <c r="W6" s="124"/>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="108"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="96"/>
+      <c r="R6" s="96"/>
+      <c r="S6" s="96"/>
+      <c r="T6" s="96"/>
+      <c r="U6" s="96"/>
+      <c r="V6" s="96"/>
+      <c r="W6" s="109"/>
       <c r="X6" s="1"/>
     </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="87"/>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
+      <c r="L7" s="111"/>
+      <c r="M7" s="111"/>
+      <c r="N7" s="112"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="114"/>
+      <c r="Q7" s="114"/>
+      <c r="R7" s="114"/>
+      <c r="S7" s="114"/>
+      <c r="T7" s="114"/>
+      <c r="U7" s="114"/>
+      <c r="V7" s="114"/>
+      <c r="W7" s="115"/>
       <c r="X7" s="1"/>
     </row>
-    <row r="8" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="125" t="s">
+    <row r="8" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="105"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="106"/>
+      <c r="F8" s="106"/>
+      <c r="G8" s="106"/>
+      <c r="H8" s="106"/>
+      <c r="I8" s="106"/>
+      <c r="J8" s="106"/>
+      <c r="K8" s="106"/>
+      <c r="L8" s="106"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="107"/>
+      <c r="O8" s="103" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="126"/>
-      <c r="Q8" s="126"/>
-      <c r="R8" s="126"/>
-      <c r="S8" s="127"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="132"/>
-      <c r="W8" s="133"/>
+      <c r="P8" s="103"/>
+      <c r="Q8" s="103"/>
+      <c r="R8" s="103"/>
+      <c r="S8" s="103"/>
+      <c r="T8" s="82"/>
+      <c r="U8" s="82"/>
+      <c r="V8" s="82"/>
+      <c r="W8" s="82"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="87"/>
-      <c r="J9" s="87"/>
-      <c r="K9" s="87"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="128" t="s">
-        <v>9</v>
+      <c r="B9" s="98"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
+      <c r="M9" s="111"/>
+      <c r="N9" s="112"/>
+      <c r="O9" s="104" t="s">
+        <v>54</v>
       </c>
-      <c r="P9" s="129"/>
-      <c r="Q9" s="129"/>
-      <c r="R9" s="129"/>
-      <c r="S9" s="130"/>
-      <c r="T9" s="88" t="s">
-        <v>10</v>
+      <c r="P9" s="104"/>
+      <c r="Q9" s="104"/>
+      <c r="R9" s="104"/>
+      <c r="S9" s="104"/>
+      <c r="T9" s="97" t="s">
+        <v>53</v>
       </c>
-      <c r="U9" s="89"/>
-      <c r="V9" s="89"/>
-      <c r="W9" s="90"/>
+      <c r="U9" s="97"/>
+      <c r="V9" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="W9" s="97"/>
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="128" t="s">
-        <v>11</v>
+      <c r="A10" s="108"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="96"/>
+      <c r="E10" s="96"/>
+      <c r="F10" s="96"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="96"/>
+      <c r="K10" s="96"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="96"/>
+      <c r="N10" s="109"/>
+      <c r="O10" s="104" t="s">
+        <v>9</v>
       </c>
-      <c r="P10" s="129"/>
-      <c r="Q10" s="129"/>
-      <c r="R10" s="129"/>
-      <c r="S10" s="130"/>
-      <c r="T10" s="134"/>
-      <c r="U10" s="135"/>
-      <c r="V10" s="135"/>
-      <c r="W10" s="136"/>
+      <c r="P10" s="104"/>
+      <c r="Q10" s="104"/>
+      <c r="R10" s="104"/>
+      <c r="S10" s="104"/>
+      <c r="T10" s="102"/>
+      <c r="U10" s="102"/>
+      <c r="V10" s="102"/>
+      <c r="W10" s="102"/>
       <c r="X10" s="6"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="77" t="s">
-        <v>12</v>
+      <c r="A11" s="98" t="s">
+        <v>10</v>
       </c>
-      <c r="B11" s="79"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="87"/>
-      <c r="M11" s="67"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="83" t="s">
-        <v>13</v>
+      <c r="B11" s="98"/>
+      <c r="C11" s="110"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="111"/>
+      <c r="K11" s="111"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="112"/>
+      <c r="O11" s="104" t="s">
+        <v>11</v>
       </c>
-      <c r="P11" s="84"/>
-      <c r="Q11" s="84"/>
-      <c r="R11" s="84"/>
-      <c r="S11" s="85"/>
-      <c r="T11" s="104"/>
-      <c r="U11" s="105"/>
-      <c r="V11" s="105"/>
-      <c r="W11" s="106"/>
+      <c r="P11" s="104"/>
+      <c r="Q11" s="104"/>
+      <c r="R11" s="104"/>
+      <c r="S11" s="104"/>
+      <c r="T11" s="102"/>
+      <c r="U11" s="102"/>
+      <c r="V11" s="102"/>
+      <c r="W11" s="102"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="1:24" ht="7.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
+    <row r="12" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="116"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="116"/>
+      <c r="R12" s="116"/>
+      <c r="S12" s="116"/>
+      <c r="T12" s="116"/>
+      <c r="U12" s="116"/>
+      <c r="V12" s="116"/>
+      <c r="W12" s="116"/>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="31.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="97" t="s">
+      <c r="A13" s="86"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="92" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
+      <c r="F13" s="93"/>
+      <c r="G13" s="94" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="95"/>
+      <c r="I13" s="95"/>
+      <c r="J13" s="95"/>
+      <c r="K13" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="99" t="s">
-        <v>15</v>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
+      <c r="N13" s="79"/>
+      <c r="O13" s="80" t="s">
+        <v>39</v>
       </c>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="116" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="118"/>
-      <c r="O13" s="119" t="s">
-        <v>42</v>
-      </c>
-      <c r="P13" s="120"/>
-      <c r="Q13" s="120"/>
-      <c r="R13" s="120"/>
-      <c r="S13" s="120"/>
-      <c r="T13" s="120"/>
-      <c r="U13" s="121"/>
+      <c r="P13" s="80"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="80"/>
+      <c r="S13" s="80"/>
+      <c r="T13" s="80"/>
+      <c r="U13" s="80"/>
+      <c r="V13" s="80"/>
+      <c r="W13" s="80"/>
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="D14" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="H14" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="29" t="s">
-        <v>52</v>
+      <c r="J14" s="57" t="s">
+        <v>50</v>
       </c>
-      <c r="E14" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="25" t="s">
+      <c r="K14" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="27" t="s">
+      <c r="L14" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="M14" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="43" t="s">
+      <c r="N14" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="44" t="s">
+      <c r="O14" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="M14" s="44" t="s">
-        <v>25</v>
+      <c r="Q14" s="63" t="s">
+        <v>40</v>
       </c>
-      <c r="N14" s="45" t="s">
-        <v>26</v>
+      <c r="R14" s="63" t="s">
+        <v>41</v>
       </c>
-      <c r="O14" s="20" t="s">
-        <v>47</v>
+      <c r="S14" s="63" t="s">
+        <v>42</v>
       </c>
-      <c r="P14" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q14" s="13" t="s">
+      <c r="T14" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="R14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="S14" s="13" t="s">
+      <c r="U14" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="T14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="U14" s="65" t="s">
-        <v>48</v>
-      </c>
+      <c r="V14" s="81"/>
+      <c r="W14" s="64"/>
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="53"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="22"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="82"/>
+      <c r="V15" s="82"/>
+      <c r="W15" s="64"/>
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="49"/>
-      <c r="O16" s="53"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="22"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="82"/>
+      <c r="V16" s="82"/>
+      <c r="W16" s="64"/>
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="49"/>
-      <c r="O17" s="53"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="22"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="82"/>
+      <c r="V17" s="82"/>
+      <c r="W17" s="64"/>
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="53"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="22"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="82"/>
+      <c r="V18" s="82"/>
+      <c r="W18" s="64"/>
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="47"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="54"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="64"/>
-      <c r="U19" s="24"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="82"/>
+      <c r="V19" s="82"/>
+      <c r="W19" s="64"/>
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="1:24" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="40"/>
-      <c r="R20" s="40"/>
-      <c r="S20" s="40"/>
-      <c r="T20" s="40"/>
-      <c r="U20" s="40"/>
-      <c r="V20" s="40"/>
-      <c r="W20" s="40"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="103" t="s">
-        <v>28</v>
+      <c r="A21" s="66" t="s">
+        <v>25</v>
       </c>
-      <c r="B21" s="103"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
@@ -7276,7 +7293,7 @@
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="55"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -7301,68 +7318,68 @@
       <c r="W23" s="11"/>
       <c r="X23" s="2"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="101" t="s">
+    <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101"/>
-      <c r="I24" s="101"/>
-      <c r="J24" s="101"/>
-      <c r="K24" s="101"/>
-      <c r="L24" s="101"/>
-      <c r="M24" s="101"/>
-      <c r="N24" s="101"/>
-      <c r="O24" s="101"/>
-      <c r="P24" s="101"/>
-      <c r="Q24" s="101"/>
-      <c r="R24" s="101"/>
-      <c r="S24" s="101"/>
-      <c r="T24" s="2"/>
-      <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
-      <c r="W24" s="2"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="83"/>
+      <c r="K24" s="83"/>
+      <c r="L24" s="83"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="83"/>
+      <c r="O24" s="83"/>
+      <c r="P24" s="83"/>
+      <c r="Q24" s="83"/>
+      <c r="R24" s="83"/>
+      <c r="S24" s="83"/>
+      <c r="T24" s="83"/>
+      <c r="U24" s="83"/>
+      <c r="V24" s="83"/>
+      <c r="W24" s="83"/>
       <c r="X24" s="5"/>
     </row>
     <row r="25" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="102"/>
-      <c r="B25" s="102"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="102"/>
-      <c r="E25" s="102"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="102"/>
-      <c r="H25" s="102"/>
-      <c r="I25" s="102"/>
-      <c r="J25" s="102"/>
-      <c r="K25" s="102"/>
-      <c r="L25" s="102"/>
-      <c r="M25" s="102"/>
-      <c r="N25" s="102"/>
-      <c r="O25" s="102"/>
-      <c r="P25" s="102"/>
-      <c r="Q25" s="102"/>
-      <c r="R25" s="102"/>
-      <c r="S25" s="102"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
+      <c r="A25" s="84"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="84"/>
+      <c r="H25" s="84"/>
+      <c r="I25" s="84"/>
+      <c r="J25" s="84"/>
+      <c r="K25" s="84"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="84"/>
+      <c r="N25" s="84"/>
+      <c r="O25" s="84"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="84"/>
+      <c r="R25" s="84"/>
+      <c r="S25" s="84"/>
+      <c r="T25" s="84"/>
+      <c r="U25" s="84"/>
+      <c r="V25" s="84"/>
+      <c r="W25" s="84"/>
       <c r="X25" s="4"/>
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="72" t="s">
-        <v>29</v>
+      <c r="A26" s="51" t="s">
+        <v>26</v>
       </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -7384,8 +7401,8 @@
       <c r="X26" s="5"/>
     </row>
     <row r="27" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="92"/>
-      <c r="B27" s="92"/>
+      <c r="A27" s="65"/>
+      <c r="B27" s="65"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -7409,86 +7426,86 @@
       <c r="W27" s="5"/>
     </row>
     <row r="28" spans="1:24" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="77" t="s">
-        <v>30</v>
+      <c r="A28" s="67" t="s">
+        <v>27</v>
       </c>
-      <c r="B28" s="78"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="78"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="80"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81"/>
-      <c r="K28" s="81"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="82"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="107" t="s">
-        <v>50</v>
+      <c r="B28" s="88"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="69" t="s">
+        <v>47</v>
       </c>
-      <c r="P28" s="108"/>
-      <c r="Q28" s="108"/>
-      <c r="R28" s="108"/>
-      <c r="S28" s="108"/>
-      <c r="T28" s="108"/>
-      <c r="U28" s="108"/>
-      <c r="V28" s="109"/>
-      <c r="W28" s="75"/>
+      <c r="P28" s="70"/>
+      <c r="Q28" s="70"/>
+      <c r="R28" s="70"/>
+      <c r="S28" s="70"/>
+      <c r="T28" s="70"/>
+      <c r="U28" s="70"/>
+      <c r="V28" s="71"/>
+      <c r="W28" s="52"/>
     </row>
     <row r="29" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="110"/>
-      <c r="P29" s="111"/>
-      <c r="Q29" s="111"/>
-      <c r="R29" s="111"/>
-      <c r="S29" s="111"/>
-      <c r="T29" s="111"/>
-      <c r="U29" s="111"/>
-      <c r="V29" s="112"/>
-      <c r="W29" s="75"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="72"/>
+      <c r="P29" s="73"/>
+      <c r="Q29" s="73"/>
+      <c r="R29" s="73"/>
+      <c r="S29" s="73"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="73"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="52"/>
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="77" t="s">
-        <v>31</v>
+      <c r="A30" s="67" t="s">
+        <v>28</v>
       </c>
-      <c r="B30" s="78"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="78"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="81"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="82"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="110"/>
-      <c r="P30" s="111"/>
-      <c r="Q30" s="111"/>
-      <c r="R30" s="111"/>
-      <c r="S30" s="111"/>
-      <c r="T30" s="111"/>
-      <c r="U30" s="111"/>
-      <c r="V30" s="112"/>
-      <c r="W30" s="75"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="72"/>
+      <c r="P30" s="73"/>
+      <c r="Q30" s="73"/>
+      <c r="R30" s="73"/>
+      <c r="S30" s="73"/>
+      <c r="T30" s="73"/>
+      <c r="U30" s="73"/>
+      <c r="V30" s="74"/>
+      <c r="W30" s="52"/>
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:24" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7506,48 +7523,48 @@
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
-      <c r="O31" s="110"/>
-      <c r="P31" s="111"/>
-      <c r="Q31" s="111"/>
-      <c r="R31" s="111"/>
-      <c r="S31" s="111"/>
-      <c r="T31" s="111"/>
-      <c r="U31" s="111"/>
-      <c r="V31" s="112"/>
-      <c r="W31" s="75"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="73"/>
+      <c r="Q31" s="73"/>
+      <c r="R31" s="73"/>
+      <c r="S31" s="73"/>
+      <c r="T31" s="73"/>
+      <c r="U31" s="73"/>
+      <c r="V31" s="74"/>
+      <c r="W31" s="52"/>
       <c r="X31" s="6"/>
     </row>
     <row r="32" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="77" t="s">
-        <v>32</v>
+      <c r="A32" s="67" t="s">
+        <v>29</v>
       </c>
-      <c r="B32" s="78"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="78"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="81"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81"/>
-      <c r="I32" s="81"/>
-      <c r="J32" s="81"/>
-      <c r="K32" s="81"/>
-      <c r="L32" s="81"/>
-      <c r="M32" s="82"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="110"/>
-      <c r="P32" s="111"/>
-      <c r="Q32" s="111"/>
-      <c r="R32" s="111"/>
-      <c r="S32" s="111"/>
-      <c r="T32" s="111"/>
-      <c r="U32" s="111"/>
-      <c r="V32" s="112"/>
-      <c r="W32" s="75"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="72"/>
+      <c r="P32" s="73"/>
+      <c r="Q32" s="73"/>
+      <c r="R32" s="73"/>
+      <c r="S32" s="73"/>
+      <c r="T32" s="73"/>
+      <c r="U32" s="73"/>
+      <c r="V32" s="74"/>
+      <c r="W32" s="52"/>
       <c r="X32" s="5"/>
     </row>
     <row r="33" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="92"/>
-      <c r="B33" s="92"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
@@ -7560,160 +7577,160 @@
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
-      <c r="O33" s="110"/>
-      <c r="P33" s="111"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="111"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="111"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="112"/>
-      <c r="W33" s="75"/>
+      <c r="O33" s="72"/>
+      <c r="P33" s="73"/>
+      <c r="Q33" s="73"/>
+      <c r="R33" s="73"/>
+      <c r="S33" s="73"/>
+      <c r="T33" s="73"/>
+      <c r="U33" s="73"/>
+      <c r="V33" s="74"/>
+      <c r="W33" s="52"/>
       <c r="X33" s="1"/>
     </row>
     <row r="34" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="77" t="s">
-        <v>33</v>
+      <c r="A34" s="67" t="s">
+        <v>30</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="81" t="s">
-        <v>34</v>
+      <c r="B34" s="88"/>
+      <c r="C34" s="88"/>
+      <c r="D34" s="88"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="90" t="s">
+        <v>31</v>
       </c>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="82"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="110"/>
-      <c r="P34" s="111"/>
-      <c r="Q34" s="111"/>
-      <c r="R34" s="111"/>
-      <c r="S34" s="111"/>
-      <c r="T34" s="111"/>
-      <c r="U34" s="111"/>
-      <c r="V34" s="112"/>
-      <c r="W34" s="75"/>
+      <c r="G34" s="90"/>
+      <c r="H34" s="90"/>
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="73"/>
+      <c r="S34" s="73"/>
+      <c r="T34" s="73"/>
+      <c r="U34" s="73"/>
+      <c r="V34" s="74"/>
+      <c r="W34" s="52"/>
       <c r="X34" s="3"/>
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="113"/>
-      <c r="P35" s="114"/>
-      <c r="Q35" s="114"/>
-      <c r="R35" s="114"/>
-      <c r="S35" s="114"/>
-      <c r="T35" s="114"/>
-      <c r="U35" s="114"/>
-      <c r="V35" s="115"/>
-      <c r="W35" s="75"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="76"/>
+      <c r="Q35" s="76"/>
+      <c r="R35" s="76"/>
+      <c r="S35" s="76"/>
+      <c r="T35" s="76"/>
+      <c r="U35" s="76"/>
+      <c r="V35" s="77"/>
+      <c r="W35" s="52"/>
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="77" t="s">
-        <v>49</v>
+      <c r="A36" s="67" t="s">
+        <v>46</v>
       </c>
-      <c r="B36" s="78"/>
-      <c r="C36" s="78"/>
-      <c r="D36" s="78"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="81" t="s">
-        <v>35</v>
+      <c r="B36" s="88"/>
+      <c r="C36" s="88"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="90" t="s">
+        <v>32</v>
       </c>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81"/>
-      <c r="I36" s="81"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="81"/>
-      <c r="L36" s="81"/>
-      <c r="M36" s="82"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="66"/>
-      <c r="Q36" s="66"/>
-      <c r="R36" s="66"/>
-      <c r="S36" s="66"/>
-      <c r="T36" s="66"/>
-      <c r="U36" s="66"/>
-      <c r="V36" s="66"/>
-      <c r="W36" s="66"/>
+      <c r="G36" s="90"/>
+      <c r="H36" s="90"/>
+      <c r="I36" s="90"/>
+      <c r="J36" s="90"/>
+      <c r="K36" s="90"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="91"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
+      <c r="T36" s="47"/>
+      <c r="U36" s="47"/>
+      <c r="V36" s="47"/>
+      <c r="W36" s="47"/>
       <c r="X36" s="3"/>
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="63"/>
-      <c r="R37" s="63"/>
-      <c r="S37" s="63"/>
-      <c r="T37" s="63"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="58"/>
-      <c r="W37" s="58"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="41"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+      <c r="T37" s="46"/>
+      <c r="U37" s="41"/>
+      <c r="V37" s="41"/>
+      <c r="W37" s="41"/>
       <c r="X37" s="6"/>
     </row>
     <row r="38" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="77" t="s">
-        <v>36</v>
+      <c r="A38" s="67" t="s">
+        <v>33</v>
       </c>
-      <c r="B38" s="78"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="78"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="81"/>
-      <c r="I38" s="81"/>
-      <c r="J38" s="81"/>
-      <c r="K38" s="81"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="82"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="58"/>
-      <c r="Q38" s="59"/>
-      <c r="R38" s="59"/>
-      <c r="S38" s="59"/>
-      <c r="T38" s="59"/>
-      <c r="U38" s="58"/>
-      <c r="V38" s="58"/>
-      <c r="W38" s="58"/>
+      <c r="B38" s="88"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="89"/>
+      <c r="G38" s="90"/>
+      <c r="H38" s="90"/>
+      <c r="I38" s="90"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="90"/>
+      <c r="L38" s="90"/>
+      <c r="M38" s="91"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="41"/>
+      <c r="Q38" s="42"/>
+      <c r="R38" s="42"/>
+      <c r="S38" s="42"/>
+      <c r="T38" s="42"/>
+      <c r="U38" s="41"/>
+      <c r="V38" s="41"/>
+      <c r="W38" s="41"/>
       <c r="X38" s="4"/>
     </row>
     <row r="39" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="92"/>
-      <c r="B39" s="92"/>
+      <c r="A39" s="65"/>
+      <c r="B39" s="65"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -7737,84 +7754,84 @@
       <c r="W39" s="4"/>
     </row>
     <row r="40" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="77" t="s">
-        <v>37</v>
+      <c r="A40" s="67" t="s">
+        <v>34</v>
       </c>
-      <c r="B40" s="78"/>
-      <c r="C40" s="78"/>
-      <c r="D40" s="78"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81"/>
-      <c r="I40" s="81"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="81"/>
-      <c r="M40" s="82"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="58"/>
-      <c r="Q40" s="59"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="59"/>
-      <c r="T40" s="59"/>
-      <c r="U40" s="59"/>
-      <c r="V40" s="59"/>
-      <c r="W40" s="59"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="88"/>
+      <c r="D40" s="88"/>
+      <c r="E40" s="68"/>
+      <c r="F40" s="89"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="90"/>
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="90"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="91"/>
+      <c r="N40" s="12"/>
+      <c r="O40" s="12"/>
+      <c r="P40" s="41"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="42"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="42"/>
+      <c r="V40" s="42"/>
+      <c r="W40" s="42"/>
     </row>
     <row r="41" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="58"/>
-      <c r="Q41" s="60"/>
-      <c r="R41" s="60"/>
-      <c r="S41" s="60"/>
-      <c r="T41" s="61"/>
-      <c r="U41" s="61"/>
-      <c r="V41" s="61"/>
-      <c r="W41" s="61"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="12"/>
+      <c r="P41" s="41"/>
+      <c r="Q41" s="43"/>
+      <c r="R41" s="43"/>
+      <c r="S41" s="43"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="44"/>
       <c r="X41" s="1"/>
     </row>
     <row r="42" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="77" t="s">
-        <v>38</v>
+      <c r="A42" s="67" t="s">
+        <v>35</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="79"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81"/>
-      <c r="I42" s="81"/>
-      <c r="J42" s="81"/>
-      <c r="K42" s="81"/>
-      <c r="L42" s="81"/>
-      <c r="M42" s="82"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
-      <c r="P42" s="58"/>
-      <c r="Q42" s="58"/>
-      <c r="R42" s="58"/>
-      <c r="S42" s="58"/>
-      <c r="T42" s="58"/>
-      <c r="U42" s="58"/>
-      <c r="V42" s="58"/>
-      <c r="W42" s="58"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="91"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="12"/>
+      <c r="P42" s="41"/>
+      <c r="Q42" s="41"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="41"/>
+      <c r="U42" s="41"/>
+      <c r="V42" s="41"/>
+      <c r="W42" s="41"/>
       <c r="X42" s="1"/>
     </row>
     <row r="43" spans="1:24" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7833,44 +7850,44 @@
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
-      <c r="P43" s="59"/>
-      <c r="Q43" s="59"/>
-      <c r="R43" s="59"/>
-      <c r="S43" s="59"/>
-      <c r="T43" s="59"/>
-      <c r="U43" s="62"/>
-      <c r="V43" s="62"/>
-      <c r="W43" s="62"/>
+      <c r="P43" s="42"/>
+      <c r="Q43" s="42"/>
+      <c r="R43" s="42"/>
+      <c r="S43" s="42"/>
+      <c r="T43" s="42"/>
+      <c r="U43" s="45"/>
+      <c r="V43" s="45"/>
+      <c r="W43" s="45"/>
       <c r="X43" s="6"/>
     </row>
     <row r="44" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="77" t="s">
-        <v>39</v>
+      <c r="A44" s="67" t="s">
+        <v>36</v>
       </c>
-      <c r="B44" s="78"/>
-      <c r="C44" s="78"/>
-      <c r="D44" s="78"/>
-      <c r="E44" s="79"/>
-      <c r="F44" s="81" t="s">
-        <v>34</v>
+      <c r="B44" s="88"/>
+      <c r="C44" s="88"/>
+      <c r="D44" s="88"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="90" t="s">
+        <v>31</v>
       </c>
-      <c r="G44" s="81"/>
-      <c r="H44" s="81"/>
-      <c r="I44" s="81"/>
-      <c r="J44" s="81"/>
-      <c r="K44" s="81"/>
-      <c r="L44" s="81"/>
-      <c r="M44" s="82"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="58"/>
-      <c r="Q44" s="59"/>
-      <c r="R44" s="59"/>
-      <c r="S44" s="59"/>
-      <c r="T44" s="59"/>
-      <c r="U44" s="58"/>
-      <c r="V44" s="58"/>
-      <c r="W44" s="58"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="90"/>
+      <c r="I44" s="90"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="90"/>
+      <c r="L44" s="90"/>
+      <c r="M44" s="91"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="41"/>
+      <c r="Q44" s="42"/>
+      <c r="R44" s="42"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="41"/>
+      <c r="V44" s="41"/>
+      <c r="W44" s="41"/>
       <c r="X44" s="1"/>
     </row>
     <row r="45" spans="1:24" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7889,47 +7906,47 @@
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
-      <c r="P45" s="59"/>
-      <c r="Q45" s="59"/>
-      <c r="R45" s="59"/>
-      <c r="S45" s="59"/>
-      <c r="T45" s="59"/>
-      <c r="U45" s="62"/>
-      <c r="V45" s="62"/>
-      <c r="W45" s="62"/>
+      <c r="P45" s="42"/>
+      <c r="Q45" s="42"/>
+      <c r="R45" s="42"/>
+      <c r="S45" s="42"/>
+      <c r="T45" s="42"/>
+      <c r="U45" s="45"/>
+      <c r="V45" s="45"/>
+      <c r="W45" s="45"/>
       <c r="X45" s="6"/>
     </row>
     <row r="46" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="77" t="s">
-        <v>40</v>
+      <c r="A46" s="67" t="s">
+        <v>37</v>
       </c>
-      <c r="B46" s="78"/>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
-      <c r="E46" s="79"/>
-      <c r="F46" s="81"/>
-      <c r="G46" s="81"/>
-      <c r="H46" s="81"/>
-      <c r="I46" s="81"/>
-      <c r="J46" s="81"/>
-      <c r="K46" s="81"/>
-      <c r="L46" s="81"/>
-      <c r="M46" s="82"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="14"/>
-      <c r="P46" s="58"/>
-      <c r="Q46" s="59"/>
-      <c r="R46" s="59"/>
-      <c r="S46" s="59"/>
-      <c r="T46" s="59"/>
-      <c r="U46" s="58"/>
-      <c r="V46" s="58"/>
-      <c r="W46" s="58"/>
+      <c r="B46" s="88"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="68"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="90"/>
+      <c r="H46" s="90"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
+      <c r="L46" s="90"/>
+      <c r="M46" s="91"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="41"/>
+      <c r="Q46" s="42"/>
+      <c r="R46" s="42"/>
+      <c r="S46" s="42"/>
+      <c r="T46" s="42"/>
+      <c r="U46" s="41"/>
+      <c r="V46" s="41"/>
+      <c r="W46" s="41"/>
       <c r="X46" s="5"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A47" s="93"/>
-      <c r="B47" s="93"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="85"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -7953,37 +7970,37 @@
       <c r="W47" s="5"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="X49" s="70"/>
+      <c r="X49" s="49"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A50" s="71"/>
-      <c r="B50" s="71"/>
-      <c r="C50" s="70"/>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
-      <c r="F50" s="70"/>
-      <c r="G50" s="70"/>
-      <c r="H50" s="70"/>
-      <c r="I50" s="70"/>
-      <c r="J50" s="70"/>
-      <c r="K50" s="70"/>
-      <c r="L50" s="70"/>
-      <c r="M50" s="70"/>
-      <c r="N50" s="70"/>
-      <c r="O50" s="70"/>
-      <c r="P50" s="70"/>
-      <c r="Q50" s="70"/>
-      <c r="R50" s="70"/>
-      <c r="S50" s="70"/>
-      <c r="T50" s="70"/>
-      <c r="U50" s="70"/>
-      <c r="V50" s="70"/>
-      <c r="W50" s="70"/>
+      <c r="A50" s="50"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="49"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
+      <c r="R50" s="49"/>
+      <c r="S50" s="49"/>
+      <c r="T50" s="49"/>
+      <c r="U50" s="49"/>
+      <c r="V50" s="49"/>
+      <c r="W50" s="49"/>
       <c r="X50" s="3"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A51" s="69"/>
-      <c r="B51" s="69"/>
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -8008,8 +8025,8 @@
       <c r="X51" s="4"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A52" s="69"/>
-      <c r="B52" s="69"/>
+      <c r="A52" s="48"/>
+      <c r="B52" s="48"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -8034,31 +8051,29 @@
       <c r="X52" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="A24:S25"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="O28:V35"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="O13:U13"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A42:E42"/>
-    <mergeCell ref="C5:L5"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="F28:M28"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="F30:M30"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
+  <mergeCells count="67">
+    <mergeCell ref="C5:N5"/>
+    <mergeCell ref="C7:N7"/>
+    <mergeCell ref="C9:N9"/>
+    <mergeCell ref="O7:W7"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="O5:R5"/>
+    <mergeCell ref="O11:S11"/>
+    <mergeCell ref="S5:W5"/>
+    <mergeCell ref="O8:S8"/>
+    <mergeCell ref="O9:S9"/>
+    <mergeCell ref="O10:S10"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="T9:U9"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="A6:W6"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="A3:W4"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:Q1"/>
     <mergeCell ref="F40:M40"/>
     <mergeCell ref="F42:M42"/>
     <mergeCell ref="A32:E32"/>
@@ -8075,23 +8090,35 @@
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="F36:M36"/>
     <mergeCell ref="F38:M38"/>
-    <mergeCell ref="A4:W4"/>
-    <mergeCell ref="A3:W3"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="R1:W1"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="O6:R6"/>
-    <mergeCell ref="O11:S11"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="S5:W5"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="O8:S8"/>
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="O10:S10"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="F28:M28"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="F30:M30"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="O28:V35"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="O13:W13"/>
+    <mergeCell ref="U14:V14"/>
+    <mergeCell ref="U15:V15"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="U18:V18"/>
+    <mergeCell ref="U19:V19"/>
+    <mergeCell ref="A24:W25"/>
+    <mergeCell ref="A12:W12"/>
+    <mergeCell ref="C11:N11"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -8116,7 +8143,7 @@
   <sheetData>
     <row r="20" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -8156,6 +8183,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010053FF0E117DAFE54CBE067C431C77F64B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ddc94be9275f957d0850a51c3b9dc2f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e3b77f1f-da53-454b-89e0-50f1aaf16bdf" xmlns:ns4="0c96800b-b425-4f1f-a293-d10a6021442d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62ab569f610cb4461c5cf91f59e28a04" ns3:_="" ns4:_="">
     <xsd:import namespace="e3b77f1f-da53-454b-89e0-50f1aaf16bdf"/>
@@ -8370,22 +8412,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731EC93D-EDAA-4042-9074-89EFD7834B98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0c96800b-b425-4f1f-a293-d10a6021442d"/>
+    <ds:schemaRef ds:uri="e3b77f1f-da53-454b-89e0-50f1aaf16bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13701D12-2EB7-4BC2-82FA-CDBEF2FAE45F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8402,29 +8454,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731EC93D-EDAA-4042-9074-89EFD7834B98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0c96800b-b425-4f1f-a293-d10a6021442d"/>
-    <ds:schemaRef ds:uri="e3b77f1f-da53-454b-89e0-50f1aaf16bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed Shipment Form PDF download
</commit_message>
<xml_diff>
--- a/public/files/tb-excel-form.xlsx
+++ b/public/files/tb-excel-form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Sites/localhost/ept/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DE5745-7305-2A4B-9850-49B5F1FF9597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08DE376-B2B2-6043-842D-5D0A24EBBCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="491" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,7 +954,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1246,6 +1246,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1308,24 +1314,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6620,7 +6608,7 @@
   <dimension ref="A1:X52"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="170" zoomScaleNormal="100" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:W1"/>
+      <selection activeCell="Q1" sqref="A1:W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6640,132 +6628,132 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="120" t="s">
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="121"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="121"/>
-      <c r="L1" s="121"/>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="122"/>
-      <c r="R1" s="99" t="s">
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="99"/>
-      <c r="T1" s="99"/>
-      <c r="U1" s="99"/>
-      <c r="V1" s="99"/>
-      <c r="W1" s="99"/>
+      <c r="R1" s="101"/>
+      <c r="S1" s="101"/>
+      <c r="T1" s="101"/>
+      <c r="U1" s="101"/>
+      <c r="V1" s="101"/>
+      <c r="W1" s="101"/>
     </row>
     <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="117"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
-      <c r="K2" s="118"/>
-      <c r="L2" s="118"/>
-      <c r="M2" s="118"/>
-      <c r="N2" s="118"/>
-      <c r="O2" s="118"/>
-      <c r="P2" s="118"/>
-      <c r="Q2" s="118"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="119"/>
+      <c r="A2" s="119"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="120"/>
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="120"/>
+      <c r="T2" s="120"/>
+      <c r="U2" s="120"/>
+      <c r="V2" s="120"/>
+      <c r="W2" s="121"/>
       <c r="X2" s="38"/>
     </row>
     <row r="3" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="100"/>
-      <c r="T3" s="100"/>
-      <c r="U3" s="100"/>
-      <c r="V3" s="100"/>
-      <c r="W3" s="100"/>
+      <c r="B3" s="102"/>
+      <c r="C3" s="102"/>
+      <c r="D3" s="102"/>
+      <c r="E3" s="102"/>
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="102"/>
+      <c r="J3" s="102"/>
+      <c r="K3" s="102"/>
+      <c r="L3" s="102"/>
+      <c r="M3" s="102"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="102"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="102"/>
       <c r="X3" s="38"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="100"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="100"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="102"/>
+      <c r="W4" s="102"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="110"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
-      <c r="K5" s="111"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="111"/>
-      <c r="N5" s="112"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="113"/>
+      <c r="E5" s="113"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="113"/>
+      <c r="L5" s="113"/>
+      <c r="M5" s="113"/>
+      <c r="N5" s="114"/>
       <c r="O5" s="98" t="s">
         <v>4</v>
       </c>
@@ -6781,7 +6769,7 @@
       <c r="W5" s="98"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="108"/>
+      <c r="A6" s="110"/>
       <c r="B6" s="96"/>
       <c r="C6" s="96"/>
       <c r="D6" s="96"/>
@@ -6803,59 +6791,59 @@
       <c r="T6" s="96"/>
       <c r="U6" s="96"/>
       <c r="V6" s="96"/>
-      <c r="W6" s="109"/>
+      <c r="W6" s="111"/>
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="101"/>
-      <c r="C7" s="110"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
-      <c r="M7" s="111"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="113"/>
-      <c r="P7" s="114"/>
-      <c r="Q7" s="114"/>
-      <c r="R7" s="114"/>
-      <c r="S7" s="114"/>
-      <c r="T7" s="114"/>
-      <c r="U7" s="114"/>
-      <c r="V7" s="114"/>
-      <c r="W7" s="115"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="112"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="113"/>
+      <c r="J7" s="113"/>
+      <c r="K7" s="113"/>
+      <c r="L7" s="113"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="114"/>
+      <c r="O7" s="115"/>
+      <c r="P7" s="116"/>
+      <c r="Q7" s="116"/>
+      <c r="R7" s="116"/>
+      <c r="S7" s="116"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="116"/>
+      <c r="V7" s="116"/>
+      <c r="W7" s="117"/>
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="105"/>
-      <c r="B8" s="106"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="106"/>
-      <c r="N8" s="107"/>
-      <c r="O8" s="103" t="s">
+      <c r="A8" s="107"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="108"/>
+      <c r="F8" s="108"/>
+      <c r="G8" s="108"/>
+      <c r="H8" s="108"/>
+      <c r="I8" s="108"/>
+      <c r="J8" s="108"/>
+      <c r="K8" s="108"/>
+      <c r="L8" s="108"/>
+      <c r="M8" s="108"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="103"/>
-      <c r="S8" s="103"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="105"/>
+      <c r="R8" s="105"/>
+      <c r="S8" s="105"/>
       <c r="T8" s="82"/>
       <c r="U8" s="82"/>
       <c r="V8" s="82"/>
@@ -6867,25 +6855,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="98"/>
-      <c r="C9" s="110"/>
-      <c r="D9" s="111"/>
-      <c r="E9" s="111"/>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
-      <c r="K9" s="111"/>
-      <c r="L9" s="111"/>
-      <c r="M9" s="111"/>
-      <c r="N9" s="112"/>
-      <c r="O9" s="104" t="s">
+      <c r="C9" s="112"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="113"/>
+      <c r="M9" s="113"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="106" t="s">
         <v>54</v>
       </c>
-      <c r="P9" s="104"/>
-      <c r="Q9" s="104"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
+      <c r="P9" s="106"/>
+      <c r="Q9" s="106"/>
+      <c r="R9" s="106"/>
+      <c r="S9" s="106"/>
       <c r="T9" s="97" t="s">
         <v>53</v>
       </c>
@@ -6897,7 +6885,7 @@
       <c r="X9" s="3"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="108"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="96"/>
       <c r="C10" s="96"/>
       <c r="D10" s="96"/>
@@ -6910,18 +6898,18 @@
       <c r="K10" s="96"/>
       <c r="L10" s="96"/>
       <c r="M10" s="96"/>
-      <c r="N10" s="109"/>
-      <c r="O10" s="104" t="s">
+      <c r="N10" s="111"/>
+      <c r="O10" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="104"/>
-      <c r="Q10" s="104"/>
-      <c r="R10" s="104"/>
-      <c r="S10" s="104"/>
-      <c r="T10" s="102"/>
-      <c r="U10" s="102"/>
-      <c r="V10" s="102"/>
-      <c r="W10" s="102"/>
+      <c r="P10" s="106"/>
+      <c r="Q10" s="106"/>
+      <c r="R10" s="106"/>
+      <c r="S10" s="106"/>
+      <c r="T10" s="104"/>
+      <c r="U10" s="104"/>
+      <c r="V10" s="104"/>
+      <c r="W10" s="104"/>
       <c r="X10" s="6"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6929,55 +6917,55 @@
         <v>10</v>
       </c>
       <c r="B11" s="98"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="111"/>
-      <c r="J11" s="111"/>
-      <c r="K11" s="111"/>
-      <c r="L11" s="111"/>
-      <c r="M11" s="111"/>
-      <c r="N11" s="112"/>
-      <c r="O11" s="104" t="s">
+      <c r="C11" s="112"/>
+      <c r="D11" s="113"/>
+      <c r="E11" s="113"/>
+      <c r="F11" s="113"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="113"/>
+      <c r="N11" s="114"/>
+      <c r="O11" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="104"/>
-      <c r="R11" s="104"/>
-      <c r="S11" s="104"/>
-      <c r="T11" s="102"/>
-      <c r="U11" s="102"/>
-      <c r="V11" s="102"/>
-      <c r="W11" s="102"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="106"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="106"/>
+      <c r="T11" s="104"/>
+      <c r="U11" s="104"/>
+      <c r="V11" s="104"/>
+      <c r="W11" s="104"/>
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="116"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="116"/>
-      <c r="R12" s="116"/>
-      <c r="S12" s="116"/>
-      <c r="T12" s="116"/>
-      <c r="U12" s="116"/>
-      <c r="V12" s="116"/>
-      <c r="W12" s="116"/>
+      <c r="A12" s="118"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="118"/>
+      <c r="E12" s="118"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="118"/>
+      <c r="M12" s="118"/>
+      <c r="N12" s="118"/>
+      <c r="O12" s="118"/>
+      <c r="P12" s="118"/>
+      <c r="Q12" s="118"/>
+      <c r="R12" s="118"/>
+      <c r="S12" s="118"/>
+      <c r="T12" s="118"/>
+      <c r="U12" s="118"/>
+      <c r="V12" s="118"/>
+      <c r="W12" s="118"/>
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" ht="31.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8069,11 +8057,11 @@
     <mergeCell ref="T9:U9"/>
     <mergeCell ref="A8:N8"/>
     <mergeCell ref="A6:W6"/>
-    <mergeCell ref="R1:W1"/>
     <mergeCell ref="A3:W4"/>
     <mergeCell ref="A2:W2"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:Q1"/>
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="Q1:W1"/>
     <mergeCell ref="F40:M40"/>
     <mergeCell ref="F42:M42"/>
     <mergeCell ref="A32:E32"/>

</xml_diff>

<commit_message>
Minor changes in the TB PDF Form
</commit_message>
<xml_diff>
--- a/public/files/tb-excel-form.xlsx
+++ b/public/files/tb-excel-form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Sites/localhost/ept/public/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F1C9FA-4F39-B74C-A98D-6EB9A786DDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B747BA8-AA4B-AC40-BE24-C12AD26E956C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="491" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$W$52</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$T$52</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>Country:</t>
   </si>
@@ -110,13 +110,7 @@
     <t>Rif Result</t>
   </si>
   <si>
-    <t>Uninterpretable Result</t>
-  </si>
-  <si>
     <t>Test Sample ID</t>
-  </si>
-  <si>
-    <t>Date Tested</t>
   </si>
   <si>
     <t>NOT DETECTED</t>
@@ -126,12 +120,6 @@
   </si>
   <si>
     <t>DETECTED</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> INVALID </t>
-  </si>
-  <si>
-    <t>NO RESULT</t>
   </si>
   <si>
     <t>ERROR</t>
@@ -367,6 +355,10 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Date 
+Tested</t>
+  </si>
 </sst>
 </file>
 
@@ -961,7 +953,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1060,18 +1052,6 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,12 +1112,6 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
@@ -1151,191 +1125,182 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1943,210 +1908,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="95" name="Oval 94">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00005F000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4185549" y="4161270"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>34236</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>226814</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="96" name="Oval 95">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000060000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4447486" y="4161270"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="97" name="Oval 96">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4292939" y="4068821"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>42174</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -2691,210 +2452,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="106" name="Oval 105">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4185549" y="4431145"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="107" name="Oval 106">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4455424" y="4431145"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="108" name="Oval 107">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4725299" y="4431145"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>42174</xdr:colOff>
       <xdr:row>16</xdr:row>
@@ -3439,210 +2996,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="117" name="Oval 116">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4185549" y="4701020"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="118" name="Oval 117">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000076000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4455424" y="4701020"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="119" name="Oval 118">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000077000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4725299" y="4701020"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>42174</xdr:colOff>
       <xdr:row>17</xdr:row>
@@ -4187,210 +3540,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="128" name="Oval 127">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000080000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4185549" y="4970895"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="129" name="Oval 128">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000081000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4455424" y="4970895"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="130" name="Oval 129">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000082000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4725299" y="4970895"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>42174</xdr:colOff>
       <xdr:row>18</xdr:row>
@@ -4935,210 +4084,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="139" name="Oval 138">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4185549" y="5240770"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="140" name="Oval 139">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4455424" y="5240770"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="141" name="Oval 140">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00008D000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4725299" y="5240770"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>42174</xdr:colOff>
       <xdr:row>14</xdr:row>
@@ -5479,13 +4424,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>59766</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>137432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>204933</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>104588</xdr:rowOff>
@@ -5547,13 +4492,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>52294</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>2572</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>371765</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>97118</xdr:rowOff>
@@ -5922,346 +4867,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1756674" y="5240770"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Oval 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E52BE8C-0920-0642-8528-A99CF296CD97}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4292939" y="4068821"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Oval 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D709FF2-61A6-C341-A132-8ADC9540D20F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4292939" y="4337763"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Oval 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EBD989C-7129-224C-A859-2D8FD028E6E9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4292939" y="4606704"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Oval 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D9BD1EA-9410-2A4B-AABF-0D05AF080CD8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4292939" y="4875645"/>
-          <a:ext cx="192578" cy="166255"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>42174</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>49645</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>234752</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Oval 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDCD683B-5B08-5F41-A714-2B970322E804}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4292939" y="5144586"/>
           <a:ext cx="192578" cy="166255"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -6627,472 +5232,426 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X52"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="170" zoomScaleNormal="100" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="Q1" sqref="A1:W1"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A9" zoomScale="170" zoomScaleNormal="100" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="14" width="3.5" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" customWidth="1"/>
-    <col min="16" max="16" width="6" customWidth="1"/>
-    <col min="17" max="17" width="6.1640625" customWidth="1"/>
-    <col min="18" max="18" width="5.83203125" customWidth="1"/>
-    <col min="19" max="19" width="4.33203125" customWidth="1"/>
-    <col min="20" max="20" width="8" customWidth="1"/>
-    <col min="21" max="21" width="5.5" customWidth="1"/>
-    <col min="22" max="22" width="3.6640625" customWidth="1"/>
-    <col min="23" max="23" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="3.5" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" customWidth="1"/>
+    <col min="10" max="11" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" customWidth="1"/>
+    <col min="16" max="16" width="6.1640625" customWidth="1"/>
+    <col min="17" max="17" width="8" customWidth="1"/>
+    <col min="18" max="18" width="5.5" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="124" t="s">
+    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="85" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
+    </row>
+    <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="82"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="34"/>
+    </row>
+    <row r="3" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="81" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="O3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="81"/>
+      <c r="R3" s="81"/>
+      <c r="S3" s="81"/>
+      <c r="T3" s="81"/>
+      <c r="U3" s="34"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="81"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+    </row>
+    <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="95"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="73"/>
+      <c r="R5" s="73"/>
+      <c r="S5" s="73"/>
+      <c r="T5" s="73"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="71"/>
+      <c r="Q6" s="71"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="71"/>
+      <c r="T6" s="72"/>
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="95"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
+      <c r="R7" s="68"/>
+      <c r="S7" s="68"/>
+      <c r="T7" s="69"/>
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="75"/>
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="73"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="73"/>
+      <c r="N9" s="73"/>
+      <c r="O9" s="73"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="R9" s="77"/>
+      <c r="S9" s="77" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="124"/>
-      <c r="G1" s="124"/>
-      <c r="H1" s="125" t="s">
-        <v>0</v>
+      <c r="T9" s="77"/>
+      <c r="U9" s="3"/>
+    </row>
+    <row r="10" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="70"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="73" t="s">
+        <v>9</v>
       </c>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="125"/>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="126" t="s">
-        <v>1</v>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="76"/>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="6"/>
+    </row>
+    <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="73" t="s">
+        <v>10</v>
       </c>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="73" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="76"/>
+      <c r="R11" s="76"/>
+      <c r="S11" s="76"/>
+      <c r="T11" s="76"/>
+      <c r="U11" s="1"/>
     </row>
-    <row r="2" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="98"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
-      <c r="N2" s="99"/>
-      <c r="O2" s="99"/>
-      <c r="P2" s="99"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="99"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="38"/>
+    <row r="12" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="116"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
+      <c r="F12" s="116"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
+      <c r="J12" s="116"/>
+      <c r="K12" s="116"/>
+      <c r="L12" s="116"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
+      <c r="O12" s="116"/>
+      <c r="P12" s="116"/>
+      <c r="Q12" s="116"/>
+      <c r="R12" s="116"/>
+      <c r="S12" s="116"/>
+      <c r="T12" s="116"/>
+      <c r="U12" s="1"/>
     </row>
-    <row r="3" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="86" t="s">
-        <v>2</v>
+    <row r="13" spans="1:21" ht="31.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="96"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="99" t="s">
+        <v>12</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="86"/>
-      <c r="T3" s="86"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
-      <c r="X3" s="38"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="100"/>
+      <c r="G13" s="101" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="102"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="74"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="74"/>
+      <c r="T13" s="74"/>
+      <c r="U13" s="1"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="86"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="86"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="86"/>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="86"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="86"/>
-    </row>
-    <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="85" t="s">
-        <v>3</v>
+    <row r="14" spans="1:21" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>14</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="91"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="93"/>
-      <c r="O5" s="85" t="s">
-        <v>4</v>
-      </c>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85" t="s">
-        <v>5</v>
-      </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="89"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
-      <c r="N6" s="84"/>
-      <c r="O6" s="84"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
-      <c r="T6" s="84"/>
-      <c r="U6" s="84"/>
-      <c r="V6" s="84"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="1"/>
-    </row>
-    <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="85" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="92"/>
-      <c r="N7" s="93"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="95"/>
-      <c r="R7" s="95"/>
-      <c r="S7" s="95"/>
-      <c r="T7" s="95"/>
-      <c r="U7" s="95"/>
-      <c r="V7" s="95"/>
-      <c r="W7" s="96"/>
-      <c r="X7" s="1"/>
-    </row>
-    <row r="8" spans="1:24" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="101"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="102"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="102"/>
-      <c r="I8" s="102"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="102"/>
-      <c r="L8" s="102"/>
-      <c r="M8" s="102"/>
-      <c r="N8" s="103"/>
-      <c r="O8" s="69" t="s">
-        <v>7</v>
-      </c>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
-      <c r="T8" s="104"/>
-      <c r="U8" s="104"/>
-      <c r="V8" s="104"/>
-      <c r="W8" s="104"/>
-      <c r="X8" s="1"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" s="85" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="91"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92"/>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
-      <c r="N9" s="93"/>
-      <c r="O9" s="85" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="105" t="s">
-        <v>52</v>
-      </c>
-      <c r="U9" s="105"/>
-      <c r="V9" s="105" t="s">
+      <c r="B14" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="W9" s="105"/>
-      <c r="X9" s="3"/>
-    </row>
-    <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="89"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="84"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="85" t="s">
-        <v>9</v>
+      <c r="C14" s="49" t="s">
+        <v>15</v>
       </c>
-      <c r="P10" s="85"/>
-      <c r="Q10" s="85"/>
-      <c r="R10" s="85"/>
-      <c r="S10" s="85"/>
-      <c r="T10" s="88"/>
-      <c r="U10" s="88"/>
-      <c r="V10" s="88"/>
-      <c r="W10" s="88"/>
-      <c r="X10" s="6"/>
-    </row>
-    <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="85" t="s">
-        <v>10</v>
+      <c r="D14" s="50" t="s">
+        <v>17</v>
       </c>
-      <c r="B11" s="85"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="92"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
-      <c r="M11" s="92"/>
-      <c r="N11" s="93"/>
-      <c r="O11" s="85" t="s">
-        <v>11</v>
+      <c r="E14" s="50" t="s">
+        <v>44</v>
       </c>
-      <c r="P11" s="85"/>
-      <c r="Q11" s="85"/>
-      <c r="R11" s="85"/>
-      <c r="S11" s="85"/>
-      <c r="T11" s="88"/>
-      <c r="U11" s="88"/>
-      <c r="V11" s="88"/>
-      <c r="W11" s="88"/>
-      <c r="X11" s="1"/>
-    </row>
-    <row r="12" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="97"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="97"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="97"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="97"/>
-      <c r="L12" s="97"/>
-      <c r="M12" s="97"/>
-      <c r="N12" s="97"/>
-      <c r="O12" s="97"/>
-      <c r="P12" s="97"/>
-      <c r="Q12" s="97"/>
-      <c r="R12" s="97"/>
-      <c r="S12" s="97"/>
-      <c r="T12" s="97"/>
-      <c r="U12" s="97"/>
-      <c r="V12" s="97"/>
-      <c r="W12" s="97"/>
-      <c r="X12" s="1"/>
-    </row>
-    <row r="13" spans="1:24" ht="31.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="80" t="s">
-        <v>12</v>
+      <c r="F14" s="50" t="s">
+        <v>18</v>
       </c>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="82" t="s">
-        <v>13</v>
+      <c r="G14" s="51" t="s">
+        <v>16</v>
       </c>
-      <c r="H13" s="83"/>
-      <c r="I13" s="83"/>
-      <c r="J13" s="83"/>
-      <c r="K13" s="67" t="s">
-        <v>14</v>
+      <c r="H14" s="52" t="s">
+        <v>15</v>
       </c>
-      <c r="L13" s="68"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
-      <c r="O13" s="69" t="s">
+      <c r="I14" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="53" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="L14" s="57" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="O14" s="57" t="s">
+        <v>37</v>
+      </c>
+      <c r="P14" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q14" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="P13" s="69"/>
-      <c r="Q13" s="69"/>
-      <c r="R13" s="69"/>
-      <c r="S13" s="69"/>
-      <c r="T13" s="69"/>
-      <c r="U13" s="69"/>
-      <c r="V13" s="69"/>
-      <c r="W13" s="69"/>
-      <c r="X13" s="1"/>
-    </row>
-    <row r="14" spans="1:24" ht="84" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="K14" s="58" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="59" t="s">
-        <v>21</v>
-      </c>
-      <c r="M14" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="O14" s="63" t="s">
-        <v>44</v>
-      </c>
-      <c r="P14" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q14" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="R14" s="63" t="s">
+      <c r="R14" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="S14" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="T14" s="63" t="s">
-        <v>43</v>
-      </c>
-      <c r="U14" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="V14" s="70"/>
-      <c r="W14" s="64"/>
-      <c r="X14" s="1"/>
+      <c r="S14" s="113"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="14"/>
       <c r="C15" s="21"/>
@@ -7103,22 +5662,19 @@
       <c r="H15" s="26"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="61"/>
+      <c r="K15" s="55"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="71"/>
-      <c r="V15" s="71"/>
-      <c r="W15" s="64"/>
-      <c r="X15" s="1"/>
+      <c r="R15" s="75"/>
+      <c r="S15" s="75"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="16"/>
       <c r="C16" s="21"/>
@@ -7129,22 +5685,19 @@
       <c r="H16" s="26"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="61"/>
+      <c r="K16" s="55"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="71"/>
-      <c r="V16" s="71"/>
-      <c r="W16" s="64"/>
-      <c r="X16" s="1"/>
+      <c r="R16" s="75"/>
+      <c r="S16" s="75"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="16"/>
       <c r="C17" s="21"/>
@@ -7155,22 +5708,19 @@
       <c r="H17" s="26"/>
       <c r="I17" s="27"/>
       <c r="J17" s="27"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="61"/>
+      <c r="K17" s="55"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="71"/>
-      <c r="V17" s="71"/>
-      <c r="W17" s="64"/>
-      <c r="X17" s="1"/>
+      <c r="R17" s="75"/>
+      <c r="S17" s="75"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="1"/>
     </row>
-    <row r="18" spans="1:24" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="16"/>
       <c r="C18" s="21"/>
@@ -7181,22 +5731,19 @@
       <c r="H18" s="26"/>
       <c r="I18" s="27"/>
       <c r="J18" s="27"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="61"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="71"/>
-      <c r="V18" s="71"/>
-      <c r="W18" s="64"/>
-      <c r="X18" s="1"/>
+      <c r="R18" s="75"/>
+      <c r="S18" s="75"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="1"/>
     </row>
-    <row r="19" spans="1:24" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="21.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
       <c r="B19" s="17"/>
       <c r="C19" s="23"/>
@@ -7207,22 +5754,19 @@
       <c r="H19" s="29"/>
       <c r="I19" s="30"/>
       <c r="J19" s="30"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="37"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="62"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="71"/>
-      <c r="V19" s="71"/>
-      <c r="W19" s="64"/>
-      <c r="X19" s="1"/>
+      <c r="R19" s="75"/>
+      <c r="S19" s="75"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="1"/>
     </row>
-    <row r="20" spans="1:24" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="32"/>
@@ -7233,26 +5777,23 @@
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
       <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
       <c r="Q20" s="31"/>
       <c r="R20" s="31"/>
       <c r="S20" s="31"/>
       <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="1"/>
+      <c r="U20" s="1"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="66" t="s">
-        <v>25</v>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="103" t="s">
+        <v>21</v>
       </c>
-      <c r="B21" s="66"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -7271,12 +5812,9 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
-      <c r="W21" s="9"/>
-      <c r="X21" s="1"/>
+      <c r="U21" s="1"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -7297,13 +5835,10 @@
       <c r="R22" s="11"/>
       <c r="S22" s="11"/>
       <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="1"/>
+      <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" s="35"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -7323,73 +5858,64 @@
       <c r="R23" s="11"/>
       <c r="S23" s="11"/>
       <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="2"/>
+      <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="72" t="s">
-        <v>50</v>
+    <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="114" t="s">
+        <v>46</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="72"/>
-      <c r="L24" s="72"/>
-      <c r="M24" s="72"/>
-      <c r="N24" s="72"/>
-      <c r="O24" s="72"/>
-      <c r="P24" s="72"/>
-      <c r="Q24" s="72"/>
-      <c r="R24" s="72"/>
-      <c r="S24" s="72"/>
-      <c r="T24" s="72"/>
-      <c r="U24" s="72"/>
-      <c r="V24" s="72"/>
-      <c r="W24" s="72"/>
-      <c r="X24" s="5"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="114"/>
+      <c r="E24" s="114"/>
+      <c r="F24" s="114"/>
+      <c r="G24" s="114"/>
+      <c r="H24" s="114"/>
+      <c r="I24" s="114"/>
+      <c r="J24" s="114"/>
+      <c r="K24" s="114"/>
+      <c r="L24" s="114"/>
+      <c r="M24" s="114"/>
+      <c r="N24" s="114"/>
+      <c r="O24" s="114"/>
+      <c r="P24" s="114"/>
+      <c r="Q24" s="114"/>
+      <c r="R24" s="114"/>
+      <c r="S24" s="114"/>
+      <c r="T24" s="114"/>
+      <c r="U24" s="5"/>
     </row>
-    <row r="25" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="73"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="73"/>
-      <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="73"/>
-      <c r="Q25" s="73"/>
-      <c r="R25" s="73"/>
-      <c r="S25" s="73"/>
-      <c r="T25" s="73"/>
-      <c r="U25" s="73"/>
-      <c r="V25" s="73"/>
-      <c r="W25" s="73"/>
-      <c r="X25" s="4"/>
+    <row r="25" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="115"/>
+      <c r="B25" s="115"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="115"/>
+      <c r="J25" s="115"/>
+      <c r="K25" s="115"/>
+      <c r="L25" s="115"/>
+      <c r="M25" s="115"/>
+      <c r="N25" s="115"/>
+      <c r="O25" s="115"/>
+      <c r="P25" s="115"/>
+      <c r="Q25" s="115"/>
+      <c r="R25" s="115"/>
+      <c r="S25" s="115"/>
+      <c r="T25" s="115"/>
+      <c r="U25" s="4"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="51" t="s">
-        <v>26</v>
+    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>22</v>
       </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -7405,14 +5931,11 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="5"/>
+      <c r="U26" s="5"/>
     </row>
-    <row r="27" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65"/>
-      <c r="B27" s="65"/>
+    <row r="27" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="98"/>
+      <c r="B27" s="98"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -7431,40 +5954,34 @@
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
     </row>
-    <row r="28" spans="1:24" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="106" t="s">
-        <v>27</v>
+    <row r="28" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="90" t="s">
+        <v>23</v>
       </c>
-      <c r="B28" s="107"/>
-      <c r="C28" s="107"/>
-      <c r="D28" s="107"/>
-      <c r="E28" s="108"/>
-      <c r="F28" s="77"/>
-      <c r="G28" s="78"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="78"/>
-      <c r="J28" s="78"/>
-      <c r="K28" s="78"/>
-      <c r="L28" s="78"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="115" t="s">
-        <v>54</v>
+      <c r="B28" s="91"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="88"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="104" t="s">
+        <v>50</v>
       </c>
-      <c r="P28" s="116"/>
-      <c r="Q28" s="116"/>
-      <c r="R28" s="116"/>
-      <c r="S28" s="116"/>
-      <c r="T28" s="116"/>
-      <c r="U28" s="116"/>
-      <c r="V28" s="117"/>
-      <c r="W28" s="52"/>
+      <c r="M28" s="105"/>
+      <c r="N28" s="105"/>
+      <c r="O28" s="105"/>
+      <c r="P28" s="105"/>
+      <c r="Q28" s="105"/>
+      <c r="R28" s="105"/>
+      <c r="S28" s="106"/>
+      <c r="T28" s="48"/>
     </row>
-    <row r="29" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -7476,49 +5993,43 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="118"/>
-      <c r="P29" s="119"/>
-      <c r="Q29" s="119"/>
-      <c r="R29" s="119"/>
-      <c r="S29" s="119"/>
-      <c r="T29" s="119"/>
-      <c r="U29" s="119"/>
-      <c r="V29" s="120"/>
-      <c r="W29" s="52"/>
-      <c r="X29" s="1"/>
+      <c r="L29" s="107"/>
+      <c r="M29" s="108"/>
+      <c r="N29" s="108"/>
+      <c r="O29" s="108"/>
+      <c r="P29" s="108"/>
+      <c r="Q29" s="108"/>
+      <c r="R29" s="108"/>
+      <c r="S29" s="109"/>
+      <c r="T29" s="48"/>
+      <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="1:24" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="106" t="s">
-        <v>28</v>
+    <row r="30" spans="1:21" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="90" t="s">
+        <v>24</v>
       </c>
-      <c r="B30" s="107"/>
-      <c r="C30" s="107"/>
-      <c r="D30" s="107"/>
-      <c r="E30" s="108"/>
-      <c r="F30" s="78"/>
-      <c r="G30" s="78"/>
-      <c r="H30" s="78"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="78"/>
-      <c r="M30" s="79"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="118"/>
-      <c r="P30" s="119"/>
-      <c r="Q30" s="119"/>
-      <c r="R30" s="119"/>
-      <c r="S30" s="119"/>
-      <c r="T30" s="119"/>
-      <c r="U30" s="119"/>
-      <c r="V30" s="120"/>
-      <c r="W30" s="52"/>
-      <c r="X30" s="1"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="89"/>
+      <c r="G30" s="89"/>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="107"/>
+      <c r="M30" s="108"/>
+      <c r="N30" s="108"/>
+      <c r="O30" s="108"/>
+      <c r="P30" s="108"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="108"/>
+      <c r="S30" s="109"/>
+      <c r="T30" s="48"/>
+      <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="1:24" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="8"/>
@@ -7530,166 +6041,148 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="118"/>
-      <c r="P31" s="119"/>
-      <c r="Q31" s="119"/>
-      <c r="R31" s="119"/>
-      <c r="S31" s="119"/>
-      <c r="T31" s="119"/>
-      <c r="U31" s="119"/>
-      <c r="V31" s="120"/>
-      <c r="W31" s="52"/>
-      <c r="X31" s="6"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="108"/>
+      <c r="N31" s="108"/>
+      <c r="O31" s="108"/>
+      <c r="P31" s="108"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="108"/>
+      <c r="S31" s="109"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="6"/>
     </row>
-    <row r="32" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="106" t="s">
-        <v>29</v>
+    <row r="32" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="90" t="s">
+        <v>25</v>
       </c>
-      <c r="B32" s="107"/>
-      <c r="C32" s="107"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="108"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="79"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="118"/>
-      <c r="P32" s="119"/>
-      <c r="Q32" s="119"/>
-      <c r="R32" s="119"/>
-      <c r="S32" s="119"/>
-      <c r="T32" s="119"/>
-      <c r="U32" s="119"/>
-      <c r="V32" s="120"/>
-      <c r="W32" s="52"/>
-      <c r="X32" s="5"/>
+      <c r="B32" s="91"/>
+      <c r="C32" s="91"/>
+      <c r="D32" s="91"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="89"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="107"/>
+      <c r="M32" s="108"/>
+      <c r="N32" s="108"/>
+      <c r="O32" s="108"/>
+      <c r="P32" s="108"/>
+      <c r="Q32" s="108"/>
+      <c r="R32" s="108"/>
+      <c r="S32" s="109"/>
+      <c r="T32" s="48"/>
+      <c r="U32" s="5"/>
     </row>
-    <row r="33" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="109"/>
-      <c r="B33" s="109"/>
-      <c r="C33" s="110"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="110"/>
+    <row r="33" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="93"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="118"/>
-      <c r="P33" s="119"/>
-      <c r="Q33" s="119"/>
-      <c r="R33" s="119"/>
-      <c r="S33" s="119"/>
-      <c r="T33" s="119"/>
-      <c r="U33" s="119"/>
-      <c r="V33" s="120"/>
-      <c r="W33" s="52"/>
-      <c r="X33" s="1"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="108"/>
+      <c r="O33" s="108"/>
+      <c r="P33" s="108"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="108"/>
+      <c r="S33" s="109"/>
+      <c r="T33" s="48"/>
+      <c r="U33" s="1"/>
     </row>
-    <row r="34" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="106" t="s">
-        <v>30</v>
+    <row r="34" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="90" t="s">
+        <v>26</v>
       </c>
-      <c r="B34" s="107"/>
-      <c r="C34" s="107"/>
-      <c r="D34" s="107"/>
-      <c r="E34" s="108"/>
-      <c r="F34" s="78" t="s">
-        <v>31</v>
+      <c r="B34" s="91"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="91"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="89" t="s">
+        <v>27</v>
       </c>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="78"/>
-      <c r="M34" s="79"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="118"/>
-      <c r="P34" s="119"/>
-      <c r="Q34" s="119"/>
-      <c r="R34" s="119"/>
-      <c r="S34" s="119"/>
-      <c r="T34" s="119"/>
-      <c r="U34" s="119"/>
-      <c r="V34" s="120"/>
-      <c r="W34" s="52"/>
-      <c r="X34" s="3"/>
+      <c r="G34" s="89"/>
+      <c r="H34" s="89"/>
+      <c r="I34" s="89"/>
+      <c r="J34" s="89"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="107"/>
+      <c r="M34" s="108"/>
+      <c r="N34" s="108"/>
+      <c r="O34" s="108"/>
+      <c r="P34" s="108"/>
+      <c r="Q34" s="108"/>
+      <c r="R34" s="108"/>
+      <c r="S34" s="109"/>
+      <c r="T34" s="48"/>
+      <c r="U34" s="3"/>
     </row>
-    <row r="35" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="111"/>
-      <c r="B35" s="111"/>
-      <c r="C35" s="111"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
+    <row r="35" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="121"/>
-      <c r="P35" s="122"/>
-      <c r="Q35" s="122"/>
-      <c r="R35" s="122"/>
-      <c r="S35" s="122"/>
-      <c r="T35" s="122"/>
-      <c r="U35" s="122"/>
-      <c r="V35" s="123"/>
-      <c r="W35" s="52"/>
-      <c r="X35" s="1"/>
+      <c r="L35" s="110"/>
+      <c r="M35" s="111"/>
+      <c r="N35" s="111"/>
+      <c r="O35" s="111"/>
+      <c r="P35" s="111"/>
+      <c r="Q35" s="111"/>
+      <c r="R35" s="111"/>
+      <c r="S35" s="112"/>
+      <c r="T35" s="48"/>
+      <c r="U35" s="1"/>
     </row>
-    <row r="36" spans="1:24" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="106" t="s">
-        <v>46</v>
+    <row r="36" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="90" t="s">
+        <v>42</v>
       </c>
-      <c r="B36" s="107"/>
-      <c r="C36" s="107"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="108"/>
-      <c r="F36" s="78" t="s">
-        <v>32</v>
+      <c r="B36" s="91"/>
+      <c r="C36" s="91"/>
+      <c r="D36" s="91"/>
+      <c r="E36" s="92"/>
+      <c r="F36" s="89" t="s">
+        <v>28</v>
       </c>
-      <c r="G36" s="78"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="78"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="78"/>
-      <c r="M36" s="79"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="47"/>
-      <c r="Q36" s="47"/>
-      <c r="R36" s="47"/>
-      <c r="S36" s="47"/>
-      <c r="T36" s="47"/>
-      <c r="U36" s="47"/>
-      <c r="V36" s="47"/>
-      <c r="W36" s="47"/>
-      <c r="X36" s="3"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="43"/>
+      <c r="S36" s="43"/>
+      <c r="T36" s="43"/>
+      <c r="U36" s="3"/>
     </row>
-    <row r="37" spans="1:24" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="111"/>
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
+    <row r="37" spans="1:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="60"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -7697,53 +6190,47 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="41"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="41"/>
-      <c r="V37" s="41"/>
-      <c r="W37" s="41"/>
-      <c r="X37" s="6"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="42"/>
+      <c r="Q37" s="42"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="6"/>
     </row>
-    <row r="38" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="106" t="s">
-        <v>33</v>
+    <row r="38" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="90" t="s">
+        <v>29</v>
       </c>
-      <c r="B38" s="107"/>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="108"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="78"/>
-      <c r="H38" s="78"/>
-      <c r="I38" s="78"/>
-      <c r="J38" s="78"/>
-      <c r="K38" s="78"/>
-      <c r="L38" s="78"/>
-      <c r="M38" s="79"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="42"/>
-      <c r="R38" s="42"/>
-      <c r="S38" s="42"/>
-      <c r="T38" s="42"/>
-      <c r="U38" s="41"/>
-      <c r="V38" s="41"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="4"/>
+      <c r="B38" s="91"/>
+      <c r="C38" s="91"/>
+      <c r="D38" s="91"/>
+      <c r="E38" s="92"/>
+      <c r="F38" s="88"/>
+      <c r="G38" s="89"/>
+      <c r="H38" s="89"/>
+      <c r="I38" s="89"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="37"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="38"/>
+      <c r="P38" s="38"/>
+      <c r="Q38" s="38"/>
+      <c r="R38" s="37"/>
+      <c r="S38" s="37"/>
+      <c r="T38" s="37"/>
+      <c r="U38" s="4"/>
     </row>
-    <row r="39" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="109"/>
-      <c r="B39" s="109"/>
-      <c r="C39" s="112"/>
-      <c r="D39" s="112"/>
-      <c r="E39" s="112"/>
+    <row r="39" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="93"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -7759,43 +6246,37 @@
       <c r="R39" s="4"/>
       <c r="S39" s="4"/>
       <c r="T39" s="4"/>
-      <c r="U39" s="4"/>
-      <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
     </row>
-    <row r="40" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="106" t="s">
-        <v>34</v>
+    <row r="40" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="90" t="s">
+        <v>30</v>
       </c>
-      <c r="B40" s="107"/>
-      <c r="C40" s="107"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="108"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="78"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="78"/>
-      <c r="J40" s="78"/>
-      <c r="K40" s="78"/>
-      <c r="L40" s="78"/>
-      <c r="M40" s="79"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="12"/>
-      <c r="P40" s="41"/>
-      <c r="Q40" s="42"/>
-      <c r="R40" s="42"/>
-      <c r="S40" s="42"/>
-      <c r="T40" s="42"/>
-      <c r="U40" s="42"/>
-      <c r="V40" s="42"/>
-      <c r="W40" s="42"/>
+      <c r="B40" s="91"/>
+      <c r="C40" s="91"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="92"/>
+      <c r="F40" s="88"/>
+      <c r="G40" s="89"/>
+      <c r="H40" s="89"/>
+      <c r="I40" s="89"/>
+      <c r="J40" s="89"/>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12"/>
+      <c r="M40" s="37"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="38"/>
+      <c r="T40" s="38"/>
     </row>
-    <row r="41" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="111"/>
-      <c r="B41" s="111"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="111"/>
-      <c r="E41" s="111"/>
+    <row r="41" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="60"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="12"/>
       <c r="G41" s="12"/>
       <c r="H41" s="12"/>
@@ -7803,53 +6284,47 @@
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
       <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="41"/>
-      <c r="Q41" s="43"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="43"/>
-      <c r="T41" s="44"/>
-      <c r="U41" s="44"/>
-      <c r="V41" s="44"/>
-      <c r="W41" s="44"/>
-      <c r="X41" s="1"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
+      <c r="P41" s="39"/>
+      <c r="Q41" s="40"/>
+      <c r="R41" s="40"/>
+      <c r="S41" s="40"/>
+      <c r="T41" s="40"/>
+      <c r="U41" s="1"/>
     </row>
-    <row r="42" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="106" t="s">
-        <v>35</v>
+    <row r="42" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="90" t="s">
+        <v>31</v>
       </c>
-      <c r="B42" s="107"/>
-      <c r="C42" s="107"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="108"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="78"/>
-      <c r="J42" s="78"/>
-      <c r="K42" s="78"/>
-      <c r="L42" s="78"/>
-      <c r="M42" s="79"/>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="41"/>
-      <c r="Q42" s="41"/>
-      <c r="R42" s="41"/>
-      <c r="S42" s="41"/>
-      <c r="T42" s="41"/>
-      <c r="U42" s="41"/>
-      <c r="V42" s="41"/>
-      <c r="W42" s="41"/>
-      <c r="X42" s="1"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="92"/>
+      <c r="F42" s="88"/>
+      <c r="G42" s="89"/>
+      <c r="H42" s="89"/>
+      <c r="I42" s="89"/>
+      <c r="J42" s="89"/>
+      <c r="K42" s="12"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
+      <c r="O42" s="37"/>
+      <c r="P42" s="37"/>
+      <c r="Q42" s="37"/>
+      <c r="R42" s="37"/>
+      <c r="S42" s="37"/>
+      <c r="T42" s="37"/>
+      <c r="U42" s="1"/>
     </row>
-    <row r="43" spans="1:24" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="113"/>
-      <c r="B43" s="113"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="114"/>
+    <row r="43" spans="1:21" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="62"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
@@ -7857,55 +6332,49 @@
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="42"/>
-      <c r="Q43" s="42"/>
-      <c r="R43" s="42"/>
-      <c r="S43" s="42"/>
-      <c r="T43" s="42"/>
-      <c r="U43" s="45"/>
-      <c r="V43" s="45"/>
-      <c r="W43" s="45"/>
-      <c r="X43" s="6"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="41"/>
+      <c r="S43" s="41"/>
+      <c r="T43" s="41"/>
+      <c r="U43" s="6"/>
     </row>
-    <row r="44" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="106" t="s">
-        <v>36</v>
+    <row r="44" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="90" t="s">
+        <v>32</v>
       </c>
-      <c r="B44" s="107"/>
-      <c r="C44" s="107"/>
-      <c r="D44" s="107"/>
-      <c r="E44" s="108"/>
-      <c r="F44" s="78" t="s">
-        <v>31</v>
+      <c r="B44" s="91"/>
+      <c r="C44" s="91"/>
+      <c r="D44" s="91"/>
+      <c r="E44" s="92"/>
+      <c r="F44" s="89" t="s">
+        <v>27</v>
       </c>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="78"/>
-      <c r="M44" s="79"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="41"/>
-      <c r="Q44" s="42"/>
-      <c r="R44" s="42"/>
-      <c r="S44" s="42"/>
-      <c r="T44" s="42"/>
-      <c r="U44" s="41"/>
-      <c r="V44" s="41"/>
-      <c r="W44" s="41"/>
-      <c r="X44" s="1"/>
+      <c r="G44" s="89"/>
+      <c r="H44" s="89"/>
+      <c r="I44" s="89"/>
+      <c r="J44" s="89"/>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12"/>
+      <c r="M44" s="37"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="37"/>
+      <c r="S44" s="37"/>
+      <c r="T44" s="37"/>
+      <c r="U44" s="1"/>
     </row>
-    <row r="45" spans="1:24" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="113"/>
-      <c r="B45" s="113"/>
-      <c r="C45" s="114"/>
-      <c r="D45" s="114"/>
-      <c r="E45" s="114"/>
+    <row r="45" spans="1:21" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="62"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="63"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
@@ -7913,50 +6382,44 @@
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="42"/>
-      <c r="Q45" s="42"/>
-      <c r="R45" s="42"/>
-      <c r="S45" s="42"/>
-      <c r="T45" s="42"/>
-      <c r="U45" s="45"/>
-      <c r="V45" s="45"/>
-      <c r="W45" s="45"/>
-      <c r="X45" s="6"/>
+      <c r="M45" s="38"/>
+      <c r="N45" s="38"/>
+      <c r="O45" s="38"/>
+      <c r="P45" s="38"/>
+      <c r="Q45" s="38"/>
+      <c r="R45" s="41"/>
+      <c r="S45" s="41"/>
+      <c r="T45" s="41"/>
+      <c r="U45" s="6"/>
     </row>
-    <row r="46" spans="1:24" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="106" t="s">
-        <v>37</v>
+    <row r="46" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="90" t="s">
+        <v>33</v>
       </c>
-      <c r="B46" s="107"/>
-      <c r="C46" s="107"/>
-      <c r="D46" s="107"/>
-      <c r="E46" s="108"/>
-      <c r="F46" s="78"/>
-      <c r="G46" s="78"/>
-      <c r="H46" s="78"/>
-      <c r="I46" s="78"/>
-      <c r="J46" s="78"/>
-      <c r="K46" s="78"/>
-      <c r="L46" s="78"/>
-      <c r="M46" s="79"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="41"/>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="42"/>
-      <c r="S46" s="42"/>
-      <c r="T46" s="42"/>
-      <c r="U46" s="41"/>
-      <c r="V46" s="41"/>
-      <c r="W46" s="41"/>
-      <c r="X46" s="5"/>
+      <c r="B46" s="91"/>
+      <c r="C46" s="91"/>
+      <c r="D46" s="91"/>
+      <c r="E46" s="92"/>
+      <c r="F46" s="89"/>
+      <c r="G46" s="89"/>
+      <c r="H46" s="89"/>
+      <c r="I46" s="89"/>
+      <c r="J46" s="89"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="38"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="38"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="5"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A47" s="74"/>
-      <c r="B47" s="74"/>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" s="94"/>
+      <c r="B47" s="94"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -7975,42 +6438,36 @@
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5"/>
-      <c r="W47" s="5"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="X49" s="49"/>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="U49" s="45"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A50" s="50"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="49"/>
-      <c r="K50" s="49"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="49"/>
-      <c r="O50" s="49"/>
-      <c r="P50" s="49"/>
-      <c r="Q50" s="49"/>
-      <c r="R50" s="49"/>
-      <c r="S50" s="49"/>
-      <c r="T50" s="49"/>
-      <c r="U50" s="49"/>
-      <c r="V50" s="49"/>
-      <c r="W50" s="49"/>
-      <c r="X50" s="3"/>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A50" s="46"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="45"/>
+      <c r="N50" s="45"/>
+      <c r="O50" s="45"/>
+      <c r="P50" s="45"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="45"/>
+      <c r="S50" s="45"/>
+      <c r="T50" s="45"/>
+      <c r="U50" s="3"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A51" s="48"/>
-      <c r="B51" s="48"/>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -8029,14 +6486,11 @@
       <c r="R51" s="3"/>
       <c r="S51" s="3"/>
       <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="4"/>
+      <c r="U51" s="4"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A52" s="48"/>
-      <c r="B52" s="48"/>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -8056,50 +6510,24 @@
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
-      <c r="V52" s="4"/>
-      <c r="W52" s="4"/>
-      <c r="X52" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="C5:N5"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C9:N9"/>
-    <mergeCell ref="O7:W7"/>
-    <mergeCell ref="A10:N10"/>
-    <mergeCell ref="O5:R5"/>
-    <mergeCell ref="O11:S11"/>
-    <mergeCell ref="S5:W5"/>
-    <mergeCell ref="O8:S8"/>
-    <mergeCell ref="O9:S9"/>
-    <mergeCell ref="O10:S10"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="T9:U9"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="A6:W6"/>
-    <mergeCell ref="A3:W4"/>
-    <mergeCell ref="A2:W2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:P1"/>
-    <mergeCell ref="Q1:W1"/>
-    <mergeCell ref="F40:M40"/>
-    <mergeCell ref="F42:M42"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="F32:M32"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="F46:M46"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="F44:M44"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="F34:M34"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="F36:M36"/>
-    <mergeCell ref="F38:M38"/>
+  <mergeCells count="66">
+    <mergeCell ref="L28:S35"/>
+    <mergeCell ref="L13:T13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="A24:T25"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="F30:J30"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A5:B5"/>
@@ -8108,27 +6536,49 @@
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:E28"/>
-    <mergeCell ref="F28:M28"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="F30:M30"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
     <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="T11:W11"/>
-    <mergeCell ref="O28:V35"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="O13:W13"/>
-    <mergeCell ref="U14:V14"/>
-    <mergeCell ref="U15:V15"/>
-    <mergeCell ref="U16:V16"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="U18:V18"/>
-    <mergeCell ref="U19:V19"/>
-    <mergeCell ref="A24:W25"/>
-    <mergeCell ref="A12:W12"/>
-    <mergeCell ref="C11:N11"/>
+    <mergeCell ref="A12:T12"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="F40:J40"/>
+    <mergeCell ref="F42:J42"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="F32:J32"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="F46:J46"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="F44:J44"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="F34:J34"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="F38:J38"/>
+    <mergeCell ref="A3:T4"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="A6:T6"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="L7:T7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="A8:K8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -8153,7 +6603,7 @@
   <sheetData>
     <row r="20" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -8193,21 +6643,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010053FF0E117DAFE54CBE067C431C77F64B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ddc94be9275f957d0850a51c3b9dc2f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e3b77f1f-da53-454b-89e0-50f1aaf16bdf" xmlns:ns4="0c96800b-b425-4f1f-a293-d10a6021442d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62ab569f610cb4461c5cf91f59e28a04" ns3:_="" ns4:_="">
     <xsd:import namespace="e3b77f1f-da53-454b-89e0-50f1aaf16bdf"/>
@@ -8422,32 +6857,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731EC93D-EDAA-4042-9074-89EFD7834B98}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0c96800b-b425-4f1f-a293-d10a6021442d"/>
-    <ds:schemaRef ds:uri="e3b77f1f-da53-454b-89e0-50f1aaf16bdf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13701D12-2EB7-4BC2-82FA-CDBEF2FAE45F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8464,4 +6889,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731EC93D-EDAA-4042-9074-89EFD7834B98}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0c96800b-b425-4f1f-a293-d10a6021442d"/>
+    <ds:schemaRef ds:uri="e3b77f1f-da53-454b-89e0-50f1aaf16bdf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Minor edits to the TB response form
</commit_message>
<xml_diff>
--- a/public/files/tb-excel-form.xlsx
+++ b/public/files/tb-excel-form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitdugar/Sites/localhost/ept/public/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B747BA8-AA4B-AC40-BE24-C12AD26E956C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0751776C-ADF7-6A42-A2C2-A4CA190C3C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" tabRatio="491" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,38 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">Submission Due Date: </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Instructions:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Fill in the circles below corresponding to the results from testing each sample provided. Document the error code in the Error Code column for tests resulting in error. Record the cycle thresholds (Ct) in the cells provided for all successful tests.  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fill information on back of form for records.</t>
-    </r>
   </si>
   <si>
     <t>Name of Site</t>
@@ -298,14 +266,6 @@
     </r>
   </si>
   <si>
-    <t>MTB/RIF Probe D
-/
-Ultra SPC</t>
-  </si>
-  <si>
-    <t>Gene-Xpert Module Number</t>
-  </si>
-  <si>
     <t xml:space="preserve">Monthly maintenance done by:     Date / Technologist </t>
   </si>
   <si>
@@ -325,9 +285,6 @@
   </si>
   <si>
     <t xml:space="preserve">MTB/RIF             </t>
-  </si>
-  <si>
-    <t>Assay (Tick One)</t>
   </si>
   <si>
     <r>
@@ -358,6 +315,49 @@
   <si>
     <t>Date 
 Tested</t>
+  </si>
+  <si>
+    <t>Probe D
+/
+SPC</t>
+  </si>
+  <si>
+    <t>Xpert Module Number</t>
+  </si>
+  <si>
+    <t>Assay (Circle One)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Instructions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Fill in the spaces below corresponding to the results from testing each sample provided. Document the error code in the Error Code column for tests resulting in error. Record the cycle thresholds (Ct) in the cells provided for all successful tests.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fill information on back of form for records.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1140,6 +1140,105 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1149,6 +1248,42 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1158,30 +1293,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1190,117 +1301,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5234,8 +5234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A9" zoomScale="170" zoomScaleNormal="100" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A46" zoomScale="170" zoomScaleNormal="100" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5259,328 +5259,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
-        <v>43</v>
+      <c r="A1" s="104" t="s">
+        <v>40</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="86" t="s">
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="104"/>
+      <c r="H1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="87" t="s">
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
     </row>
     <row r="2" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="82"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="84"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="103"/>
       <c r="U2" s="34"/>
     </row>
     <row r="3" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="81" t="s">
-        <v>2</v>
+      <c r="A3" s="100" t="s">
+        <v>51</v>
       </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="O3" s="81"/>
-      <c r="P3" s="81"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="81"/>
-      <c r="S3" s="81"/>
-      <c r="T3" s="81"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
       <c r="U3" s="34"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="81"/>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="100"/>
+      <c r="O4" s="100"/>
+      <c r="P4" s="100"/>
+      <c r="Q4" s="100"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="100"/>
+      <c r="T4" s="100"/>
     </row>
     <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="91"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="99"/>
+      <c r="L5" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="65"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="73" t="s">
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="73"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="73"/>
-      <c r="T5" s="73"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="90"/>
+      <c r="T5" s="90"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="70"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="71"/>
-      <c r="T6" s="72"/>
+      <c r="A6" s="109"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="110"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="110"/>
+      <c r="L6" s="110"/>
+      <c r="M6" s="110"/>
+      <c r="N6" s="110"/>
+      <c r="O6" s="110"/>
+      <c r="P6" s="110"/>
+      <c r="Q6" s="110"/>
+      <c r="R6" s="110"/>
+      <c r="S6" s="110"/>
+      <c r="T6" s="111"/>
       <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="73" t="s">
-        <v>6</v>
+      <c r="A7" s="90" t="s">
+        <v>5</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
-      <c r="S7" s="68"/>
-      <c r="T7" s="69"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="112"/>
+      <c r="M7" s="113"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="113"/>
+      <c r="S7" s="113"/>
+      <c r="T7" s="114"/>
       <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="78"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="80"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
+      <c r="F8" s="116"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
+      <c r="I8" s="116"/>
+      <c r="J8" s="116"/>
+      <c r="K8" s="117"/>
       <c r="L8" s="74" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M8" s="74"/>
       <c r="N8" s="74"/>
       <c r="O8" s="74"/>
       <c r="P8" s="74"/>
-      <c r="Q8" s="75"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="75"/>
-      <c r="T8" s="75"/>
+      <c r="Q8" s="76"/>
+      <c r="R8" s="76"/>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
       <c r="U8" s="1"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="73" t="s">
-        <v>8</v>
+      <c r="A9" s="90" t="s">
+        <v>7</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="73" t="s">
-        <v>49</v>
+      <c r="B9" s="90"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="90" t="s">
+        <v>50</v>
       </c>
-      <c r="M9" s="73"/>
-      <c r="N9" s="73"/>
-      <c r="O9" s="73"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="77" t="s">
-        <v>48</v>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="108" t="s">
+        <v>45</v>
       </c>
-      <c r="R9" s="77"/>
-      <c r="S9" s="77" t="s">
-        <v>47</v>
+      <c r="R9" s="108"/>
+      <c r="S9" s="108" t="s">
+        <v>44</v>
       </c>
-      <c r="T9" s="77"/>
+      <c r="T9" s="108"/>
       <c r="U9" s="3"/>
     </row>
     <row r="10" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="70"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="71"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="73" t="s">
-        <v>9</v>
+      <c r="A10" s="109"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="110"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
+      <c r="I10" s="110"/>
+      <c r="J10" s="110"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="90" t="s">
+        <v>8</v>
       </c>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
-      <c r="S10" s="76"/>
-      <c r="T10" s="76"/>
+      <c r="M10" s="90"/>
+      <c r="N10" s="90"/>
+      <c r="O10" s="90"/>
+      <c r="P10" s="90"/>
+      <c r="Q10" s="107"/>
+      <c r="R10" s="107"/>
+      <c r="S10" s="107"/>
+      <c r="T10" s="107"/>
       <c r="U10" s="6"/>
     </row>
     <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="90"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="99"/>
+      <c r="L11" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="M11" s="73"/>
-      <c r="N11" s="73"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="76"/>
-      <c r="S11" s="76"/>
-      <c r="T11" s="76"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
       <c r="U11" s="1"/>
     </row>
     <row r="12" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
-      <c r="L12" s="116"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
-      <c r="O12" s="116"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="116"/>
-      <c r="R12" s="116"/>
-      <c r="S12" s="116"/>
-      <c r="T12" s="116"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="96"/>
+      <c r="M12" s="96"/>
+      <c r="N12" s="96"/>
+      <c r="O12" s="96"/>
+      <c r="P12" s="96"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="96"/>
+      <c r="S12" s="96"/>
+      <c r="T12" s="96"/>
       <c r="U12" s="1"/>
     </row>
     <row r="13" spans="1:21" ht="31.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="99" t="s">
+      <c r="A13" s="92"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="102"/>
-      <c r="I13" s="102"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="117"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="87"/>
+      <c r="J13" s="87"/>
+      <c r="K13" s="64"/>
       <c r="L13" s="74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M13" s="74"/>
       <c r="N13" s="74"/>
@@ -5594,60 +5594,60 @@
     </row>
     <row r="14" spans="1:21" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>51</v>
+      <c r="D14" s="50" t="s">
+        <v>16</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="E14" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="50" t="s">
-        <v>17</v>
+      <c r="H14" s="52" t="s">
+        <v>14</v>
       </c>
-      <c r="E14" s="50" t="s">
-        <v>44</v>
+      <c r="I14" s="53" t="s">
+        <v>16</v>
       </c>
-      <c r="F14" s="50" t="s">
+      <c r="J14" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="51" t="s">
-        <v>16</v>
+      <c r="L14" s="57" t="s">
+        <v>48</v>
       </c>
-      <c r="H14" s="52" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="53" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="54" t="s">
+      <c r="M14" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="57" t="s">
-        <v>40</v>
+      <c r="N14" s="57" t="s">
+        <v>35</v>
       </c>
-      <c r="M14" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="57" t="s">
+      <c r="O14" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="O14" s="57" t="s">
+      <c r="P14" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="P14" s="57" t="s">
+      <c r="Q14" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="57" t="s">
-        <v>39</v>
+      <c r="R14" s="75" t="s">
+        <v>49</v>
       </c>
-      <c r="R14" s="113" t="s">
-        <v>41</v>
-      </c>
-      <c r="S14" s="113"/>
+      <c r="S14" s="75"/>
       <c r="T14" s="58"/>
       <c r="U14" s="1"/>
     </row>
@@ -5669,8 +5669,8 @@
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
-      <c r="R15" s="75"/>
-      <c r="S15" s="75"/>
+      <c r="R15" s="76"/>
+      <c r="S15" s="76"/>
       <c r="T15" s="58"/>
       <c r="U15" s="1"/>
     </row>
@@ -5692,8 +5692,8 @@
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
-      <c r="R16" s="75"/>
-      <c r="S16" s="75"/>
+      <c r="R16" s="76"/>
+      <c r="S16" s="76"/>
       <c r="T16" s="58"/>
       <c r="U16" s="1"/>
     </row>
@@ -5715,8 +5715,8 @@
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
-      <c r="R17" s="75"/>
-      <c r="S17" s="75"/>
+      <c r="R17" s="76"/>
+      <c r="S17" s="76"/>
       <c r="T17" s="58"/>
       <c r="U17" s="1"/>
     </row>
@@ -5738,8 +5738,8 @@
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
+      <c r="R18" s="76"/>
+      <c r="S18" s="76"/>
       <c r="T18" s="58"/>
       <c r="U18" s="1"/>
     </row>
@@ -5761,8 +5761,8 @@
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
+      <c r="R19" s="76"/>
+      <c r="S19" s="76"/>
       <c r="T19" s="58"/>
       <c r="U19" s="1"/>
     </row>
@@ -5790,10 +5790,10 @@
       <c r="U20" s="1"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="103" t="s">
-        <v>21</v>
+      <c r="A21" s="88" t="s">
+        <v>20</v>
       </c>
-      <c r="B21" s="103"/>
+      <c r="B21" s="88"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -5861,56 +5861,56 @@
       <c r="U23" s="2"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="114" t="s">
-        <v>46</v>
+      <c r="A24" s="77" t="s">
+        <v>43</v>
       </c>
-      <c r="B24" s="114"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="114"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="114"/>
-      <c r="P24" s="114"/>
-      <c r="Q24" s="114"/>
-      <c r="R24" s="114"/>
-      <c r="S24" s="114"/>
-      <c r="T24" s="114"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
+      <c r="I24" s="77"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="77"/>
+      <c r="L24" s="77"/>
+      <c r="M24" s="77"/>
+      <c r="N24" s="77"/>
+      <c r="O24" s="77"/>
+      <c r="P24" s="77"/>
+      <c r="Q24" s="77"/>
+      <c r="R24" s="77"/>
+      <c r="S24" s="77"/>
+      <c r="T24" s="77"/>
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:21" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="115"/>
-      <c r="B25" s="115"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="115"/>
-      <c r="E25" s="115"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="115"/>
-      <c r="H25" s="115"/>
-      <c r="I25" s="115"/>
-      <c r="J25" s="115"/>
-      <c r="K25" s="115"/>
-      <c r="L25" s="115"/>
-      <c r="M25" s="115"/>
-      <c r="N25" s="115"/>
-      <c r="O25" s="115"/>
-      <c r="P25" s="115"/>
-      <c r="Q25" s="115"/>
-      <c r="R25" s="115"/>
-      <c r="S25" s="115"/>
-      <c r="T25" s="115"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
       <c r="U25" s="4"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="47"/>
       <c r="C26" s="36"/>
@@ -5934,8 +5934,8 @@
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="98"/>
-      <c r="B27" s="98"/>
+      <c r="A27" s="94"/>
+      <c r="B27" s="94"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -5956,29 +5956,29 @@
       <c r="T27" s="5"/>
     </row>
     <row r="28" spans="1:21" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="90" t="s">
-        <v>23</v>
+      <c r="A28" s="81" t="s">
+        <v>22</v>
       </c>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="91"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="88"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="80"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
       <c r="K28" s="12"/>
-      <c r="L28" s="104" t="s">
-        <v>50</v>
+      <c r="L28" s="65" t="s">
+        <v>46</v>
       </c>
-      <c r="M28" s="105"/>
-      <c r="N28" s="105"/>
-      <c r="O28" s="105"/>
-      <c r="P28" s="105"/>
-      <c r="Q28" s="105"/>
-      <c r="R28" s="105"/>
-      <c r="S28" s="106"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
+      <c r="S28" s="67"/>
       <c r="T28" s="48"/>
     </row>
     <row r="29" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -5993,39 +5993,39 @@
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="108"/>
-      <c r="N29" s="108"/>
-      <c r="O29" s="108"/>
-      <c r="P29" s="108"/>
-      <c r="Q29" s="108"/>
-      <c r="R29" s="108"/>
-      <c r="S29" s="109"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="69"/>
+      <c r="P29" s="69"/>
+      <c r="Q29" s="69"/>
+      <c r="R29" s="69"/>
+      <c r="S29" s="70"/>
       <c r="T29" s="48"/>
       <c r="U29" s="1"/>
     </row>
     <row r="30" spans="1:21" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="90" t="s">
-        <v>24</v>
+      <c r="A30" s="81" t="s">
+        <v>23</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="91"/>
-      <c r="D30" s="91"/>
-      <c r="E30" s="92"/>
-      <c r="F30" s="89"/>
-      <c r="G30" s="89"/>
-      <c r="H30" s="89"/>
-      <c r="I30" s="89"/>
-      <c r="J30" s="89"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
+      <c r="H30" s="80"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
       <c r="K30" s="12"/>
-      <c r="L30" s="107"/>
-      <c r="M30" s="108"/>
-      <c r="N30" s="108"/>
-      <c r="O30" s="108"/>
-      <c r="P30" s="108"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="108"/>
-      <c r="S30" s="109"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
+      <c r="Q30" s="69"/>
+      <c r="R30" s="69"/>
+      <c r="S30" s="70"/>
       <c r="T30" s="48"/>
       <c r="U30" s="1"/>
     </row>
@@ -6041,45 +6041,45 @@
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
-      <c r="L31" s="107"/>
-      <c r="M31" s="108"/>
-      <c r="N31" s="108"/>
-      <c r="O31" s="108"/>
-      <c r="P31" s="108"/>
-      <c r="Q31" s="108"/>
-      <c r="R31" s="108"/>
-      <c r="S31" s="109"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="69"/>
+      <c r="R31" s="69"/>
+      <c r="S31" s="70"/>
       <c r="T31" s="48"/>
       <c r="U31" s="6"/>
     </row>
     <row r="32" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="90" t="s">
-        <v>25</v>
+      <c r="A32" s="81" t="s">
+        <v>24</v>
       </c>
-      <c r="B32" s="91"/>
-      <c r="C32" s="91"/>
-      <c r="D32" s="91"/>
-      <c r="E32" s="92"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="89"/>
-      <c r="I32" s="89"/>
-      <c r="J32" s="89"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="107"/>
-      <c r="M32" s="108"/>
-      <c r="N32" s="108"/>
-      <c r="O32" s="108"/>
-      <c r="P32" s="108"/>
-      <c r="Q32" s="108"/>
-      <c r="R32" s="108"/>
-      <c r="S32" s="109"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="69"/>
+      <c r="S32" s="70"/>
       <c r="T32" s="48"/>
       <c r="U32" s="5"/>
     </row>
     <row r="33" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="93"/>
-      <c r="B33" s="93"/>
+      <c r="A33" s="95"/>
+      <c r="B33" s="95"/>
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
@@ -6089,41 +6089,41 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="108"/>
-      <c r="N33" s="108"/>
-      <c r="O33" s="108"/>
-      <c r="P33" s="108"/>
-      <c r="Q33" s="108"/>
-      <c r="R33" s="108"/>
-      <c r="S33" s="109"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="69"/>
+      <c r="R33" s="69"/>
+      <c r="S33" s="70"/>
       <c r="T33" s="48"/>
       <c r="U33" s="1"/>
     </row>
     <row r="34" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="91"/>
-      <c r="C34" s="91"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="92"/>
-      <c r="F34" s="89" t="s">
-        <v>27</v>
-      </c>
-      <c r="G34" s="89"/>
-      <c r="H34" s="89"/>
-      <c r="I34" s="89"/>
-      <c r="J34" s="89"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="108"/>
-      <c r="N34" s="108"/>
-      <c r="O34" s="108"/>
-      <c r="P34" s="108"/>
-      <c r="Q34" s="108"/>
-      <c r="R34" s="108"/>
-      <c r="S34" s="109"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="69"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="69"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="69"/>
+      <c r="S34" s="70"/>
       <c r="T34" s="48"/>
       <c r="U34" s="3"/>
     </row>
@@ -6139,32 +6139,32 @@
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
-      <c r="L35" s="110"/>
-      <c r="M35" s="111"/>
-      <c r="N35" s="111"/>
-      <c r="O35" s="111"/>
-      <c r="P35" s="111"/>
-      <c r="Q35" s="111"/>
-      <c r="R35" s="111"/>
-      <c r="S35" s="112"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="72"/>
+      <c r="O35" s="72"/>
+      <c r="P35" s="72"/>
+      <c r="Q35" s="72"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="73"/>
       <c r="T35" s="48"/>
       <c r="U35" s="1"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="90" t="s">
-        <v>42</v>
+      <c r="A36" s="81" t="s">
+        <v>39</v>
       </c>
-      <c r="B36" s="91"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="92"/>
-      <c r="F36" s="89" t="s">
-        <v>28</v>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="80" t="s">
+        <v>27</v>
       </c>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="43"/>
@@ -6201,18 +6201,18 @@
       <c r="U37" s="6"/>
     </row>
     <row r="38" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="90" t="s">
-        <v>29</v>
+      <c r="A38" s="81" t="s">
+        <v>28</v>
       </c>
-      <c r="B38" s="91"/>
-      <c r="C38" s="91"/>
-      <c r="D38" s="91"/>
-      <c r="E38" s="92"/>
-      <c r="F38" s="88"/>
-      <c r="G38" s="89"/>
-      <c r="H38" s="89"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="37"/>
@@ -6226,8 +6226,8 @@
       <c r="U38" s="4"/>
     </row>
     <row r="39" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="93"/>
-      <c r="B39" s="93"/>
+      <c r="A39" s="95"/>
+      <c r="B39" s="95"/>
       <c r="C39" s="61"/>
       <c r="D39" s="61"/>
       <c r="E39" s="61"/>
@@ -6248,18 +6248,18 @@
       <c r="T39" s="4"/>
     </row>
     <row r="40" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="90" t="s">
-        <v>30</v>
+      <c r="A40" s="81" t="s">
+        <v>29</v>
       </c>
-      <c r="B40" s="91"/>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="92"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="89"/>
-      <c r="H40" s="89"/>
-      <c r="I40" s="89"/>
-      <c r="J40" s="89"/>
+      <c r="B40" s="82"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="80"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="37"/>
@@ -6295,18 +6295,18 @@
       <c r="U41" s="1"/>
     </row>
     <row r="42" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="90" t="s">
-        <v>31</v>
+      <c r="A42" s="81" t="s">
+        <v>30</v>
       </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
-      <c r="E42" s="92"/>
-      <c r="F42" s="88"/>
-      <c r="G42" s="89"/>
-      <c r="H42" s="89"/>
-      <c r="I42" s="89"/>
-      <c r="J42" s="89"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="83"/>
+      <c r="F42" s="79"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="80"/>
+      <c r="I42" s="80"/>
+      <c r="J42" s="80"/>
       <c r="K42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="37"/>
@@ -6343,20 +6343,20 @@
       <c r="U43" s="6"/>
     </row>
     <row r="44" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="90" t="s">
-        <v>32</v>
+      <c r="A44" s="81" t="s">
+        <v>31</v>
       </c>
-      <c r="B44" s="91"/>
-      <c r="C44" s="91"/>
-      <c r="D44" s="91"/>
-      <c r="E44" s="92"/>
-      <c r="F44" s="89" t="s">
-        <v>27</v>
+      <c r="B44" s="82"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="80" t="s">
+        <v>26</v>
       </c>
-      <c r="G44" s="89"/>
-      <c r="H44" s="89"/>
-      <c r="I44" s="89"/>
-      <c r="J44" s="89"/>
+      <c r="G44" s="80"/>
+      <c r="H44" s="80"/>
+      <c r="I44" s="80"/>
+      <c r="J44" s="80"/>
       <c r="K44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="37"/>
@@ -6393,18 +6393,18 @@
       <c r="U45" s="6"/>
     </row>
     <row r="46" spans="1:21" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="90" t="s">
-        <v>33</v>
+      <c r="A46" s="81" t="s">
+        <v>32</v>
       </c>
-      <c r="B46" s="91"/>
-      <c r="C46" s="91"/>
-      <c r="D46" s="91"/>
-      <c r="E46" s="92"/>
-      <c r="F46" s="89"/>
-      <c r="G46" s="89"/>
-      <c r="H46" s="89"/>
-      <c r="I46" s="89"/>
-      <c r="J46" s="89"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="83"/>
+      <c r="F46" s="80"/>
+      <c r="G46" s="80"/>
+      <c r="H46" s="80"/>
+      <c r="I46" s="80"/>
+      <c r="J46" s="80"/>
       <c r="K46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="37"/>
@@ -6418,8 +6418,8 @@
       <c r="U46" s="5"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="94"/>
-      <c r="B47" s="94"/>
+      <c r="A47" s="89"/>
+      <c r="B47" s="89"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
@@ -6513,21 +6513,40 @@
     </row>
   </sheetData>
   <mergeCells count="66">
-    <mergeCell ref="L28:S35"/>
-    <mergeCell ref="L13:T13"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="A24:T25"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="F30:J30"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="L5:O5"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="L11:P11"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="L9:P9"/>
+    <mergeCell ref="L10:P10"/>
+    <mergeCell ref="Q8:T8"/>
+    <mergeCell ref="Q10:T10"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="A6:T6"/>
+    <mergeCell ref="Q11:T11"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="C9:K9"/>
+    <mergeCell ref="L7:T7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A3:T4"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:T1"/>
+    <mergeCell ref="F34:J34"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="F38:J38"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="F46:J46"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="F44:J44"/>
+    <mergeCell ref="A38:E38"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A5:B5"/>
@@ -6544,41 +6563,22 @@
     <mergeCell ref="F42:J42"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="F32:J32"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="F46:J46"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="F44:J44"/>
-    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="L28:S35"/>
+    <mergeCell ref="L13:T13"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="A24:T25"/>
+    <mergeCell ref="F28:J28"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="F30:J30"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A21:B21"/>
     <mergeCell ref="A34:E34"/>
-    <mergeCell ref="F34:J34"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A36:E36"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="F38:J38"/>
-    <mergeCell ref="A3:T4"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="N1:T1"/>
-    <mergeCell ref="L11:P11"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="L9:P9"/>
-    <mergeCell ref="L10:P10"/>
-    <mergeCell ref="Q8:T8"/>
-    <mergeCell ref="Q10:T10"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="A6:T6"/>
-    <mergeCell ref="Q11:T11"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="C9:K9"/>
-    <mergeCell ref="L7:T7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="L5:O5"/>
-    <mergeCell ref="A8:K8"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6603,7 +6603,7 @@
   <sheetData>
     <row r="20" spans="9:9" x14ac:dyDescent="0.2">
       <c r="I20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -6858,18 +6858,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6892,14 +6892,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{731EC93D-EDAA-4042-9074-89EFD7834B98}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6914,4 +6906,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{406F8738-F0C1-443B-9141-D098C4F4DF72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>